<commit_message>
Changed LPW_LRL, MPW_LRL, MPW_HRL ALPHA run selections because non-hauling BEV overall costs appeared to high relative to ICE. Reduced Weight learning rate to 0 from 0.01 because when applied to the entire body cost, it dominates other learning effects, and results in 2050 ICE costs that are too low relative to BEVs. Onroad range changed to 300. Changed base_wt calculation to use glider_weight instead of curb_wt to avoid double counting battery costs. Changed bev_weight_reduction to 0.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBolon\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544DDC08-F045-4A15-8AB6-69678B9CCCDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9B4638-5336-4594-B8F1-E3DCCF63D1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" firstSheet="2" activeTab="13" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="390" yWindow="300" windowWidth="17895" windowHeight="14910" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sherwood, Todd:</t>
         </r>
@@ -87,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 enter values as integers
@@ -1351,7 +1351,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1513,19 +1513,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2112,16 +2099,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>297</v>
       </c>
@@ -2129,7 +2116,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -2137,7 +2124,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>300</v>
       </c>
@@ -2145,15 +2132,15 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>301</v>
       </c>
       <c r="B4" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>369</v>
       </c>
@@ -2161,7 +2148,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>302</v>
       </c>
@@ -2169,7 +2156,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -2177,7 +2164,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>323</v>
       </c>
@@ -2198,12 +2185,12 @@
       <selection activeCell="F1" sqref="F1:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>334</v>
       </c>
@@ -2226,7 +2213,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="str">
         <f>CONCATENATE(B2,"_",D2)</f>
         <v>unibody_0</v>
@@ -2251,7 +2238,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
         <f t="shared" ref="A3:A11" si="1">CONCATENATE(B3,"_",D3)</f>
         <v>unibody_5</v>
@@ -2276,7 +2263,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -2301,7 +2288,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -2326,7 +2313,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2351,7 +2338,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2376,7 +2363,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2401,7 +2388,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2426,7 +2413,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2451,7 +2438,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2491,15 +2478,15 @@
       <selection activeCell="F5" sqref="F5:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="34"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="34"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>365</v>
       </c>
@@ -2522,7 +2509,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>C2</f>
         <v>LDB</v>
@@ -2544,7 +2531,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
         <f>C3</f>
         <v>LRRT1</v>
@@ -2567,7 +2554,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="str">
         <f>C4</f>
         <v>LRRT2</v>
@@ -2591,7 +2578,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="str">
         <f t="shared" ref="A5:A14" si="1">CONCATENATE(B5,"_",D5)</f>
         <v>unibody_0</v>
@@ -2616,7 +2603,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_5</v>
@@ -2642,7 +2629,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -2668,7 +2655,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -2694,7 +2681,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2720,7 +2707,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2745,7 +2732,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2771,7 +2758,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2797,7 +2784,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2823,7 +2810,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2864,9 +2851,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>366</v>
       </c>
@@ -2880,7 +2867,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>367</v>
       </c>
@@ -2895,7 +2882,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>368</v>
       </c>
@@ -2923,21 +2910,21 @@
       <selection activeCell="K51" sqref="K51:K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="181.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="181.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2975,7 +2962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>183</v>
       </c>
@@ -3013,7 +3000,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>184</v>
       </c>
@@ -3051,7 +3038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>185</v>
       </c>
@@ -3089,7 +3076,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>186</v>
       </c>
@@ -3127,7 +3114,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>193</v>
       </c>
@@ -3162,7 +3149,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>194</v>
       </c>
@@ -3197,7 +3184,7 @@
         <v>159.27502634351916</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>195</v>
       </c>
@@ -3232,7 +3219,7 @@
         <v>179.18440463645993</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>197</v>
       </c>
@@ -3267,7 +3254,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>198</v>
       </c>
@@ -3302,7 +3289,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>199</v>
       </c>
@@ -3337,7 +3324,7 @@
         <v>367.54500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
@@ -3372,7 +3359,7 @@
         <v>442.06851256369526</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>205</v>
       </c>
@@ -3410,7 +3397,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>215</v>
       </c>
@@ -3448,7 +3435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>216</v>
       </c>
@@ -3483,7 +3470,7 @@
         <v>113.57755999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>229</v>
       </c>
@@ -3518,7 +3505,7 @@
         <v>-97.21050000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>230</v>
       </c>
@@ -3553,7 +3540,7 @@
         <v>-220.98500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>241</v>
       </c>
@@ -3588,7 +3575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>265</v>
       </c>
@@ -3623,7 +3610,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>266</v>
       </c>
@@ -3658,7 +3645,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>267</v>
       </c>
@@ -3696,7 +3683,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>268</v>
       </c>
@@ -3734,7 +3721,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>269</v>
       </c>
@@ -3773,7 +3760,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>271</v>
       </c>
@@ -3808,7 +3795,7 @@
         <v>-847.59770000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>272</v>
       </c>
@@ -3843,7 +3830,7 @@
         <v>-626.61270000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>273</v>
       </c>
@@ -3878,7 +3865,7 @@
         <v>88.164999999999964</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>274</v>
       </c>
@@ -3913,7 +3900,7 @@
         <v>309.14999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>275</v>
       </c>
@@ -3948,7 +3935,7 @@
         <v>-658.79864999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>276</v>
       </c>
@@ -3983,7 +3970,7 @@
         <v>-437.81365</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>277</v>
       </c>
@@ -4018,7 +4005,7 @@
         <v>541.10772384767472</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>278</v>
       </c>
@@ -4053,7 +4040,7 @@
         <v>188.79966055354828</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>279</v>
       </c>
@@ -4088,7 +4075,7 @@
         <v>-940.23964999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>280</v>
       </c>
@@ -4123,7 +4110,7 @@
         <v>-313.62695000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>281</v>
       </c>
@@ -4158,7 +4145,7 @@
         <v>-265.93770000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>282</v>
       </c>
@@ -4193,7 +4180,7 @@
         <v>360.67500000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>283</v>
       </c>
@@ -4228,7 +4215,7 @@
         <v>592.64179278554764</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>284</v>
       </c>
@@ -4263,7 +4250,7 @@
         <v>-804.40830000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>285</v>
       </c>
@@ -4298,7 +4285,7 @@
         <v>-177.79560000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>286</v>
       </c>
@@ -4333,7 +4320,7 @@
         <v>135.83591145034848</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>287</v>
       </c>
@@ -4368,7 +4355,7 @@
         <v>-722.52935000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>288</v>
       </c>
@@ -4403,7 +4390,7 @@
         <v>-95.91664999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>289</v>
       </c>
@@ -4438,7 +4425,7 @@
         <v>217.71486145034851</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>294</v>
       </c>
@@ -4473,7 +4460,7 @@
         <v>132.72918861960008</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>295</v>
       </c>
@@ -4508,7 +4495,7 @@
         <v>192.45732349841887</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>296</v>
       </c>
@@ -4543,7 +4530,7 @@
         <v>274.95</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>297</v>
       </c>
@@ -4581,7 +4568,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>298</v>
       </c>
@@ -4619,7 +4606,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>300</v>
       </c>
@@ -4657,7 +4644,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>301</v>
       </c>
@@ -4695,7 +4682,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>302</v>
       </c>
@@ -4733,7 +4720,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>314</v>
       </c>
@@ -4765,7 +4752,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>315</v>
       </c>
@@ -4797,7 +4784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>316</v>
       </c>
@@ -4829,7 +4816,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>317</v>
       </c>
@@ -4861,7 +4848,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>320</v>
       </c>
@@ -4893,7 +4880,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>321</v>
       </c>
@@ -4925,7 +4912,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>337</v>
       </c>
@@ -4954,7 +4941,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>338</v>
       </c>
@@ -4983,7 +4970,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>339</v>
       </c>
@@ -5012,7 +4999,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>358</v>
       </c>
@@ -5041,7 +5028,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>359</v>
       </c>
@@ -5070,7 +5057,7 @@
         <v>11.875</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>360</v>
       </c>
@@ -5111,20 +5098,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ACC5D0-181B-4F4E-94F7-26883B6AC5A8}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="34" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>297</v>
       </c>
@@ -5141,7 +5128,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>386</v>
       </c>
@@ -5156,7 +5143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>389</v>
       </c>
@@ -5171,7 +5158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>387</v>
       </c>
@@ -5186,7 +5173,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -5201,7 +5188,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -5212,7 +5199,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>392</v>
       </c>
@@ -5223,7 +5210,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>251</v>
       </c>
@@ -5245,18 +5232,18 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="34" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>297</v>
       </c>
@@ -5273,7 +5260,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>377</v>
       </c>
@@ -5290,7 +5277,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -5307,7 +5294,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>379</v>
       </c>
@@ -5324,7 +5311,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>380</v>
       </c>
@@ -5355,30 +5342,30 @@
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="34" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>294</v>
       </c>
@@ -5437,7 +5424,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="str">
         <f>CONCATENATE("bev_",C2,"_",B2)</f>
         <v>bev_300_LPW_LRL</v>
@@ -5505,7 +5492,7 @@
         <v>163.65691955817854</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="str">
         <f t="shared" ref="A3:A7" si="1">CONCATENATE("bev_",C3,"_",B3)</f>
         <v>bev_300_MPW_LRL</v>
@@ -5573,7 +5560,7 @@
         <v>172.3599834464473</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="str">
         <f t="shared" si="1"/>
         <v>bev_300_LPW_HRL</v>
@@ -5641,7 +5628,7 @@
         <v>180.05754544257272</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="str">
         <f t="shared" si="1"/>
         <v>bev_300_HPW</v>
@@ -5709,7 +5696,7 @@
         <v>184.79936714697126</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="str">
         <f t="shared" si="1"/>
         <v>bev_300_MPW_HRL</v>
@@ -5777,7 +5764,7 @@
         <v>176.34808200639765</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="str">
         <f t="shared" si="1"/>
         <v>bev_300_Truck</v>
@@ -5845,8 +5832,8 @@
         <v>169.20753046813238</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="20"/>
       <c r="D9" s="13"/>
       <c r="H9" s="20"/>
@@ -5859,7 +5846,7 @@
         <v>0.22445418158725869</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>
       <c r="C10" s="21"/>
       <c r="E10" s="13"/>
@@ -5874,7 +5861,7 @@
         <v>60.602629028559839</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11" s="21"/>
       <c r="E11" s="13"/>
@@ -5885,7 +5872,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="35"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="21"/>
       <c r="E12" s="13"/>
@@ -5896,7 +5883,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="35"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
       <c r="C13" s="21"/>
       <c r="E13" s="13"/>
@@ -5907,7 +5894,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="21"/>
       <c r="D14" s="19"/>
@@ -5919,7 +5906,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="35"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="21"/>
       <c r="D15" s="19"/>
@@ -5932,7 +5919,7 @@
       <c r="K15" s="21"/>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="21"/>
       <c r="D16" s="19"/>
@@ -5945,7 +5932,7 @@
       <c r="K16" s="21"/>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="21"/>
       <c r="D17" s="19"/>
@@ -5958,7 +5945,7 @@
       <c r="K17" s="21"/>
       <c r="L17" s="35"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="21"/>
       <c r="D18" s="19"/>
@@ -5971,7 +5958,7 @@
       <c r="K18" s="21"/>
       <c r="L18" s="35"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="21"/>
       <c r="D19" s="19"/>
@@ -5984,7 +5971,7 @@
       <c r="K19" s="21"/>
       <c r="L19" s="35"/>
     </row>
-    <row r="20" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="13"/>
       <c r="C20" s="21"/>
@@ -5996,7 +5983,7 @@
       <c r="K20" s="21"/>
       <c r="L20" s="35"/>
     </row>
-    <row r="21" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
       <c r="B21" s="13"/>
       <c r="C21" s="21"/>
@@ -6008,7 +5995,7 @@
       <c r="K21" s="21"/>
       <c r="L21" s="35"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
       <c r="C22" s="21"/>
       <c r="D22" s="19"/>
@@ -6020,7 +6007,7 @@
       <c r="K22" s="21"/>
       <c r="L22" s="35"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="C23" s="21"/>
       <c r="D23" s="19"/>
@@ -6032,7 +6019,7 @@
       <c r="K23" s="21"/>
       <c r="L23" s="35"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
@@ -6040,7 +6027,7 @@
       <c r="K24" s="21"/>
       <c r="L24" s="35"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
@@ -6048,7 +6035,7 @@
       <c r="K25" s="21"/>
       <c r="L25" s="35"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
@@ -6056,7 +6043,7 @@
       <c r="K26" s="21"/>
       <c r="L26" s="35"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
@@ -6064,7 +6051,7 @@
       <c r="K27" s="21"/>
       <c r="L27" s="35"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -6086,17 +6073,17 @@
       <selection activeCell="D8" sqref="D8:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="17" t="s">
         <v>252</v>
       </c>
@@ -6144,7 +6131,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>260</v>
       </c>
@@ -6186,7 +6173,7 @@
         <v>69.219987721658612</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>260</v>
       </c>
@@ -6229,7 +6216,7 @@
         <v>66.858403643459866</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>260</v>
       </c>
@@ -6272,7 +6259,7 @@
         <v>62.107868498937762</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>260</v>
       </c>
@@ -6315,7 +6302,7 @@
         <v>60.107594658208214</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>260</v>
       </c>
@@ -6358,7 +6345,7 @@
         <v>58.444762271426534</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>260</v>
       </c>
@@ -6407,7 +6394,7 @@
         <v>103.82998158248792</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>261</v>
       </c>
@@ -6456,7 +6443,7 @@
         <v>100.2876054651898</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>261</v>
       </c>
@@ -6506,7 +6493,7 @@
         <v>93.161802748406643</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>261</v>
       </c>
@@ -6556,7 +6543,7 @@
         <v>90.161391987312328</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>261</v>
       </c>
@@ -6606,7 +6593,7 @@
         <v>87.667143407139804</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>261</v>
       </c>
@@ -6656,7 +6643,7 @@
         <v>-53.480281881786084</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>261</v>
       </c>
@@ -6706,7 +6693,7 @@
         <v>67.572665627399303</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>264</v>
       </c>
@@ -6775,7 +6762,7 @@
         <v>-80.220422822679083</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>264</v>
       </c>
@@ -6844,7 +6831,7 @@
         <v>101.35899844109895</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>264</v>
       </c>
@@ -6907,7 +6894,7 @@
         <v>101.35899844109895</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>264</v>
       </c>
@@ -6970,7 +6957,7 @@
         <v>99.754589984645364</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>264</v>
       </c>
@@ -7033,7 +7020,7 @@
         <v>95.342466729398012</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>264</v>
       </c>
@@ -7096,7 +7083,7 @@
         <v>93.336956158831043</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>264</v>
       </c>
@@ -7159,7 +7146,7 @@
         <v>85.314913876563125</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>264</v>
       </c>
@@ -7195,7 +7182,7 @@
         <v>7499.2546955683456</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>264</v>
       </c>
@@ -7231,7 +7218,7 @@
         <v>8079.4243576536282</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>264</v>
       </c>
@@ -7267,7 +7254,7 @@
         <v>8747.7579222501754</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>264</v>
       </c>
@@ -7303,7 +7290,7 @@
         <v>10316.074361911862</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>264</v>
       </c>
@@ -7339,7 +7326,7 @@
         <v>11193.802212219591</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
         <v>319</v>
       </c>
@@ -7347,7 +7334,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>245</v>
       </c>
@@ -7385,7 +7372,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C32" s="17">
         <v>0</v>
       </c>
@@ -7429,7 +7416,7 @@
         <v>103.07282791177303</v>
       </c>
     </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="17">
         <v>0.02</v>
       </c>
@@ -7473,7 +7460,7 @@
         <v>100.2876054651894</v>
       </c>
     </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="17">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7517,7 +7504,7 @@
         <v>95.759495559138685</v>
       </c>
     </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35" s="17">
         <v>0.1</v>
       </c>
@@ -7561,7 +7548,7 @@
         <v>95.759001244663736</v>
       </c>
     </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36" s="17">
         <v>0.2</v>
       </c>
@@ -7605,7 +7592,7 @@
         <v>95.759495559138685</v>
       </c>
     </row>
-    <row r="37" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="34">
         <v>0</v>
       </c>
@@ -7634,7 +7621,7 @@
         <v>6000.4061836817873</v>
       </c>
     </row>
-    <row r="38" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="34">
         <v>0.02</v>
       </c>
@@ -7663,7 +7650,7 @@
         <v>6003.804122707772</v>
       </c>
     </row>
-    <row r="39" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="34">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7692,7 +7679,7 @@
         <v>6013.1484550292289</v>
       </c>
     </row>
-    <row r="40" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="34">
         <v>0.1</v>
       </c>
@@ -7721,7 +7708,7 @@
         <v>6017.3958788117088</v>
       </c>
     </row>
-    <row r="41" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="34">
         <v>0.2</v>
       </c>
@@ -7750,7 +7737,7 @@
         <v>6034.3855739416304</v>
       </c>
     </row>
-    <row r="42" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="34">
         <v>0</v>
       </c>
@@ -7779,7 +7766,7 @@
         <v>16985.77336324126</v>
       </c>
     </row>
-    <row r="43" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="34">
         <v>0.02</v>
       </c>
@@ -7808,7 +7795,7 @@
         <v>16767.118644244714</v>
       </c>
     </row>
-    <row r="44" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="34">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7837,7 +7824,7 @@
         <v>16108.942603440479</v>
       </c>
     </row>
-    <row r="45" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="34">
         <v>0.1</v>
       </c>
@@ -7866,7 +7853,7 @@
         <v>16113.087003216284</v>
       </c>
     </row>
-    <row r="46" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="34">
         <v>0.2</v>
       </c>
@@ -7895,7 +7882,7 @@
         <v>16130.179722352881</v>
       </c>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C47" s="17" t="s">
         <v>317</v>
       </c>
@@ -7951,7 +7938,7 @@
         <v>-34.041987144201435</v>
       </c>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C48" s="17" t="s">
         <v>318</v>
       </c>
@@ -8007,7 +7994,7 @@
         <v>100.81700213237262</v>
       </c>
     </row>
-    <row r="50" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="17" t="s">
         <v>321</v>
       </c>
@@ -8031,7 +8018,7 @@
         <v>-5625.3516666666674</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C51" s="45" t="s">
         <v>322</v>
       </c>
@@ -8051,9 +8038,9 @@
       <selection activeCell="B2" sqref="B2:E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>255</v>
       </c>
@@ -8070,7 +8057,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -8087,7 +8074,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2018</v>
       </c>
@@ -8104,7 +8091,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2019</v>
       </c>
@@ -8121,7 +8108,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>2020</v>
       </c>
@@ -8138,7 +8125,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2021</v>
       </c>
@@ -8155,7 +8142,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2022</v>
       </c>
@@ -8172,7 +8159,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>2023</v>
       </c>
@@ -8189,7 +8176,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>2024</v>
       </c>
@@ -8206,7 +8193,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>2025</v>
       </c>
@@ -8223,7 +8210,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>2026</v>
       </c>
@@ -8240,7 +8227,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>2027</v>
       </c>
@@ -8257,7 +8244,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>2028</v>
       </c>
@@ -8274,7 +8261,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>2029</v>
       </c>
@@ -8291,7 +8278,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2030</v>
       </c>
@@ -8308,7 +8295,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>2031</v>
       </c>
@@ -8325,7 +8312,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2032</v>
       </c>
@@ -8342,7 +8329,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>2033</v>
       </c>
@@ -8359,7 +8346,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2034</v>
       </c>
@@ -8376,7 +8363,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2035</v>
       </c>
@@ -8393,7 +8380,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>2036</v>
       </c>
@@ -8410,7 +8397,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>2037</v>
       </c>
@@ -8427,7 +8414,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>2038</v>
       </c>
@@ -8444,7 +8431,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>2039</v>
       </c>
@@ -8461,7 +8448,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>2040</v>
       </c>
@@ -8478,7 +8465,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>2041</v>
       </c>
@@ -8495,7 +8482,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2042</v>
       </c>
@@ -8512,7 +8499,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>2043</v>
       </c>
@@ -8529,7 +8516,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>2044</v>
       </c>
@@ -8546,7 +8533,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>2045</v>
       </c>
@@ -8563,7 +8550,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>2046</v>
       </c>
@@ -8580,7 +8567,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>2047</v>
       </c>
@@ -8597,7 +8584,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>2048</v>
       </c>
@@ -8614,7 +8601,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>2049</v>
       </c>
@@ -8631,7 +8618,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>2050</v>
       </c>
@@ -8648,22 +8635,22 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
     </row>
   </sheetData>
@@ -8677,12 +8664,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="8.88671875" style="34"/>
+    <col min="2" max="3" width="8.85546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>315</v>
       </c>
@@ -8723,7 +8710,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
         <v>2020</v>
       </c>
@@ -8764,7 +8751,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>2021</v>
       </c>
@@ -8805,7 +8792,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2022</v>
       </c>
@@ -8846,7 +8833,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>2023</v>
       </c>
@@ -8887,7 +8874,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>2024</v>
       </c>
@@ -8928,7 +8915,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>2025</v>
       </c>
@@ -8969,7 +8956,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>2026</v>
       </c>
@@ -9010,7 +8997,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>2027</v>
       </c>
@@ -9051,7 +9038,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>2028</v>
       </c>
@@ -9092,7 +9079,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>2029</v>
       </c>
@@ -9133,7 +9120,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>2030</v>
       </c>
@@ -9174,7 +9161,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>2031</v>
       </c>
@@ -9215,7 +9202,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>2032</v>
       </c>
@@ -9256,7 +9243,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>2033</v>
       </c>
@@ -9297,7 +9284,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>2034</v>
       </c>
@@ -9338,7 +9325,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>2035</v>
       </c>
@@ -9379,7 +9366,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>2036</v>
       </c>
@@ -9420,7 +9407,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>2037</v>
       </c>
@@ -9461,7 +9448,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>2038</v>
       </c>
@@ -9502,7 +9489,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>2039</v>
       </c>
@@ -9543,7 +9530,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>2040</v>
       </c>
@@ -9584,7 +9571,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>2041</v>
       </c>
@@ -9625,7 +9612,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>2042</v>
       </c>
@@ -9666,7 +9653,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>2043</v>
       </c>
@@ -9707,7 +9694,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>2044</v>
       </c>
@@ -9748,7 +9735,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>2045</v>
       </c>
@@ -9789,7 +9776,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>2046</v>
       </c>
@@ -9830,7 +9817,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>2047</v>
       </c>
@@ -9871,7 +9858,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>2048</v>
       </c>
@@ -9912,7 +9899,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>2049</v>
       </c>
@@ -9953,7 +9940,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <v>2050</v>
       </c>
@@ -10008,12 +9995,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10024,7 +10011,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>193</v>
       </c>
@@ -10035,7 +10022,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -10046,7 +10033,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>195</v>
       </c>
@@ -10057,7 +10044,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10068,7 +10055,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>333</v>
       </c>
@@ -10090,9 +10077,9 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>304</v>
       </c>
@@ -10100,7 +10087,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2006</v>
       </c>
@@ -10108,7 +10095,7 @@
         <v>90.073999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2007</v>
       </c>
@@ -10116,7 +10103,7 @@
         <v>92.498000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -10124,7 +10111,7 @@
         <v>94.263999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2009</v>
       </c>
@@ -10132,7 +10119,7 @@
         <v>94.998999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2010</v>
       </c>
@@ -10140,7 +10127,7 @@
         <v>96.108999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -10148,7 +10135,7 @@
         <v>98.111999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -10156,7 +10143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -10164,7 +10151,7 @@
         <v>101.773</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -10172,7 +10159,7 @@
         <v>103.64700000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -10180,7 +10167,7 @@
         <v>104.688</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -10188,7 +10175,7 @@
         <v>105.77</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2017</v>
       </c>
@@ -10196,7 +10183,7 @@
         <v>107.795</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -10204,7 +10191,7 @@
         <v>110.38200000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -10212,7 +10199,7 @@
         <v>112.348</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>316</v>
       </c>
@@ -10231,9 +10218,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>331</v>
       </c>
@@ -10241,7 +10228,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10249,7 +10236,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10257,7 +10244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -10265,7 +10252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -10286,14 +10273,14 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="34"/>
+    <col min="1" max="1" width="22.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>297</v>
       </c>
@@ -10307,7 +10294,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>325</v>
       </c>
@@ -10322,7 +10309,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>326</v>
       </c>
@@ -10337,7 +10324,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>327</v>
       </c>
@@ -10352,7 +10339,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>330</v>
       </c>
@@ -10367,7 +10354,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>328</v>
       </c>
@@ -10382,7 +10369,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>335</v>
       </c>
@@ -10397,7 +10384,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>336</v>
       </c>
@@ -10412,7 +10399,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>337</v>
       </c>
@@ -10427,7 +10414,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>338</v>
       </c>
@@ -10442,7 +10429,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>339</v>
       </c>
@@ -10457,7 +10444,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>340</v>
       </c>
@@ -10472,7 +10459,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>341</v>
       </c>
@@ -10487,7 +10474,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
         <v>342</v>
       </c>
@@ -10502,7 +10489,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>343</v>
       </c>
@@ -10517,7 +10504,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>344</v>
       </c>
@@ -10532,7 +10519,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>345</v>
       </c>
@@ -10547,7 +10534,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>346</v>
       </c>
@@ -10562,7 +10549,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>347</v>
       </c>
@@ -10577,7 +10564,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
         <v>348</v>
       </c>
@@ -10592,7 +10579,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
         <v>349</v>
       </c>
@@ -10607,7 +10594,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
         <v>350</v>
       </c>
@@ -10622,7 +10609,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
         <v>212</v>
       </c>
@@ -10637,7 +10624,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>351</v>
       </c>
@@ -10653,7 +10640,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>352</v>
       </c>
@@ -10669,7 +10656,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
         <v>353</v>
       </c>
@@ -10685,7 +10672,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>354</v>
       </c>
@@ -10700,7 +10687,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>373</v>
       </c>
@@ -10715,7 +10702,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>374</v>
       </c>
@@ -10730,7 +10717,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>375</v>
       </c>
@@ -10745,7 +10732,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
         <v>376</v>
       </c>
@@ -10773,17 +10760,17 @@
       <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="34" customWidth="1"/>
     <col min="24" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="9.88671875" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -10878,7 +10865,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10982,7 +10969,7 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11088,7 +11075,7 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11197,7 +11184,7 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -11308,7 +11295,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11419,7 +11406,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -11530,7 +11517,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -11634,7 +11621,7 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -11740,7 +11727,7 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -11847,7 +11834,7 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -11956,7 +11943,7 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -12067,7 +12054,7 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -12178,7 +12165,7 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -12289,7 +12276,7 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -12396,7 +12383,7 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -12502,7 +12489,7 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -12615,7 +12602,7 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -12726,7 +12713,7 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -12830,7 +12817,7 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -12936,7 +12923,7 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -13040,7 +13027,7 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -13146,7 +13133,7 @@
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -13257,7 +13244,7 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -13368,7 +13355,7 @@
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -13476,7 +13463,7 @@
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -13587,7 +13574,7 @@
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -13698,7 +13685,7 @@
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -13808,7 +13795,7 @@
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -13916,7 +13903,7 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -14029,7 +14016,7 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -14160,15 +14147,15 @@
       <selection activeCell="F2" sqref="F2:F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.33203125" style="34" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="34"/>
+    <col min="1" max="1" width="21.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>364</v>
       </c>
@@ -14194,7 +14181,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="str">
         <f>CONCATENATE(B2,"_",C2,"_",D2)</f>
         <v>TRX10_FWD_LPW_LRL</v>
@@ -14222,7 +14209,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="str">
         <f t="shared" ref="A3:A7" si="1">CONCATENATE(B3,"_",C3,"_",D3)</f>
         <v>TRX10_FWD_LPW_HRL</v>
@@ -14250,7 +14237,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_LRL</v>
@@ -14278,7 +14265,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_HRL</v>
@@ -14306,7 +14293,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_HPW</v>
@@ -14334,7 +14321,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_Truck</v>
@@ -14362,7 +14349,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="str">
         <f t="shared" ref="A8:A61" si="2">CONCATENATE(B8,"_",C8,"_",D8)</f>
         <v>TRX11_FWD_LPW_LRL</v>
@@ -14391,7 +14378,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_LPW_HRL</v>
@@ -14420,7 +14407,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_LRL</v>
@@ -14449,7 +14436,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_HRL</v>
@@ -14478,7 +14465,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_HPW</v>
@@ -14507,7 +14494,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_Truck</v>
@@ -14536,7 +14523,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_LRL</v>
@@ -14565,7 +14552,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_HRL</v>
@@ -14594,7 +14581,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_LRL</v>
@@ -14623,7 +14610,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_HRL</v>
@@ -14652,7 +14639,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_HPW</v>
@@ -14681,7 +14668,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_Truck</v>
@@ -14710,7 +14697,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_LRL</v>
@@ -14739,7 +14726,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_HRL</v>
@@ -14768,7 +14755,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_LRL</v>
@@ -14797,7 +14784,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_HRL</v>
@@ -14826,7 +14813,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_HPW</v>
@@ -14855,7 +14842,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_Truck</v>
@@ -14884,7 +14871,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_LRL</v>
@@ -14913,7 +14900,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_HRL</v>
@@ -14942,7 +14929,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_LRL</v>
@@ -14971,7 +14958,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_HRL</v>
@@ -15000,7 +14987,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_HPW</v>
@@ -15029,7 +15016,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_Truck</v>
@@ -15058,7 +15045,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="str">
         <f>CONCATENATE(B32,"_",C32,"_",D32)</f>
         <v>TRX10_AWD_LPW_LRL</v>
@@ -15087,7 +15074,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="str">
         <f t="shared" ref="A33:A37" si="4">CONCATENATE(B33,"_",C33,"_",D33)</f>
         <v>TRX10_AWD_LPW_HRL</v>
@@ -15116,7 +15103,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_LRL</v>
@@ -15145,7 +15132,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_HRL</v>
@@ -15174,7 +15161,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_HPW</v>
@@ -15203,7 +15190,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_Truck</v>
@@ -15232,7 +15219,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_LRL</v>
@@ -15261,7 +15248,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_HRL</v>
@@ -15290,7 +15277,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_LRL</v>
@@ -15319,7 +15306,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_HRL</v>
@@ -15348,7 +15335,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_HPW</v>
@@ -15377,7 +15364,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_Truck</v>
@@ -15406,7 +15393,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_LRL</v>
@@ -15435,7 +15422,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_HRL</v>
@@ -15464,7 +15451,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_LRL</v>
@@ -15493,7 +15480,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_HRL</v>
@@ -15522,7 +15509,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_HPW</v>
@@ -15551,7 +15538,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_Truck</v>
@@ -15580,7 +15567,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_LRL</v>
@@ -15609,7 +15596,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_HRL</v>
@@ -15638,7 +15625,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_LRL</v>
@@ -15667,7 +15654,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_HRL</v>
@@ -15696,7 +15683,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_HPW</v>
@@ -15725,7 +15712,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_Truck</v>
@@ -15754,7 +15741,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_LRL</v>
@@ -15783,7 +15770,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_HRL</v>
@@ -15812,7 +15799,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_LRL</v>
@@ -15841,7 +15828,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_HRL</v>
@@ -15870,7 +15857,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_HPW</v>
@@ -15899,7 +15886,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="34" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_Truck</v>
@@ -15928,7 +15915,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="34" t="str">
         <f>CONCATENATE(B62,"_",C62,"_",D62)</f>
         <v>TRX10_RWD_LPW_LRL</v>
@@ -15957,7 +15944,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="str">
         <f t="shared" ref="A63:A67" si="7">CONCATENATE(B63,"_",C63,"_",D63)</f>
         <v>TRX10_RWD_LPW_HRL</v>
@@ -15986,7 +15973,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_LRL</v>
@@ -16015,7 +16002,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="34" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_HRL</v>
@@ -16044,7 +16031,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_HPW</v>
@@ -16073,7 +16060,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_Truck</v>
@@ -16102,7 +16089,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="str">
         <f t="shared" ref="A68:A91" si="9">CONCATENATE(B68,"_",C68,"_",D68)</f>
         <v>TRX11_RWD_LPW_LRL</v>
@@ -16131,7 +16118,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_LPW_HRL</v>
@@ -16160,7 +16147,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_LRL</v>
@@ -16189,7 +16176,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_HRL</v>
@@ -16218,7 +16205,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_HPW</v>
@@ -16247,7 +16234,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_Truck</v>
@@ -16276,7 +16263,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_LRL</v>
@@ -16305,7 +16292,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_HRL</v>
@@ -16334,7 +16321,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_LRL</v>
@@ -16363,7 +16350,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_HRL</v>
@@ -16392,7 +16379,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_HPW</v>
@@ -16421,7 +16408,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_Truck</v>
@@ -16450,7 +16437,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_LRL</v>
@@ -16479,7 +16466,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_HRL</v>
@@ -16508,7 +16495,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_LRL</v>
@@ -16537,7 +16524,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_HRL</v>
@@ -16566,7 +16553,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_HPW</v>
@@ -16595,7 +16582,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_Truck</v>
@@ -16624,7 +16611,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_LRL</v>
@@ -16653,7 +16640,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_HRL</v>
@@ -16682,7 +16669,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_LRL</v>
@@ -16711,7 +16698,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_HRL</v>
@@ -16740,7 +16727,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_HPW</v>
@@ -16769,7 +16756,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="34" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_Truck</v>
@@ -16813,13 +16800,13 @@
       <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>220</v>
       </c>
@@ -16833,7 +16820,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -16848,7 +16835,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -16863,7 +16850,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -16878,7 +16865,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -16893,7 +16880,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -16908,7 +16895,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>223</v>
       </c>
@@ -16923,7 +16910,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -16938,7 +16925,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -16953,7 +16940,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -16968,7 +16955,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -16983,7 +16970,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -16998,7 +16985,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>229</v>
       </c>
@@ -17013,7 +17000,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>230</v>
       </c>
@@ -17028,7 +17015,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -17043,7 +17030,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>232</v>
       </c>
@@ -17058,7 +17045,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>216</v>
       </c>
@@ -17074,7 +17061,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>217</v>
       </c>
@@ -17090,7 +17077,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>218</v>
       </c>
@@ -17106,7 +17093,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>219</v>
       </c>
@@ -17122,7 +17109,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -17138,7 +17125,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -17167,14 +17154,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="34"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="34"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>355</v>
       </c>
@@ -17194,7 +17181,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <v>0</v>
       </c>
@@ -17215,7 +17202,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <v>1</v>
       </c>
@@ -17237,7 +17224,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <v>2</v>
       </c>
@@ -17270,19 +17257,19 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>366</v>
       </c>
@@ -17305,7 +17292,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>367</v>
       </c>
@@ -17329,7 +17316,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>368</v>
       </c>

</xml_diff>

<commit_message>
In alpha_package_costs.py: Add ability to calc PEV weight costs differently from ICE. Add dollar basis and kWh_gross to detailed_cost output files. Add generate_cost_cloud_file to SetInputs class so that the cloud file isn't generated unless requested.
In alpha_package_costs_module_inputs.xlsx:
Add weight_pev worksheet.
Update PEV curve data to latest.

BEV ALPHA file is now a mish-mash of real ALPHA runs and values we have created to get results that make more sense.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B712F-53BB-4F39-B9A2-F42A20725F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86C7397-3E15-4257-9154-007F57A113A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" activeTab="2" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="trans" sheetId="2" r:id="rId7"/>
     <sheet name="accessories" sheetId="3" r:id="rId8"/>
     <sheet name="start-stop" sheetId="5" r:id="rId9"/>
-    <sheet name="weight" sheetId="4" r:id="rId10"/>
-    <sheet name="aero" sheetId="6" r:id="rId11"/>
-    <sheet name="nonaero" sheetId="9" r:id="rId12"/>
-    <sheet name="ac" sheetId="17" r:id="rId13"/>
-    <sheet name="et_dmc" sheetId="7" r:id="rId14"/>
+    <sheet name="weight_ice" sheetId="4" r:id="rId10"/>
+    <sheet name="weight_pev" sheetId="22" r:id="rId11"/>
+    <sheet name="aero" sheetId="6" r:id="rId12"/>
+    <sheet name="nonaero" sheetId="9" r:id="rId13"/>
+    <sheet name="ac" sheetId="17" r:id="rId14"/>
+    <sheet name="et_dmc" sheetId="7" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">aero!$B$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">nonaero!$C$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">aero!$B$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">nonaero!$C$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">trans!$A$1:$H$91</definedName>
     <definedName name="AWD_scaler">inputs_workbook!$B$6</definedName>
     <definedName name="Markup">inputs_workbook!$B$1</definedName>
@@ -57,8 +58,52 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sherwood, Todd</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C4D4E348-B3CC-4315-8C9C-4D45F7A7FFE0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sherwood, Todd:
+From MSa: 20210406_1732</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+For battery cost, at various annual production volumes:
+50K: $/gross kWh = -0.00011558x3 + 0.03260786x2 - 3.23269439x + 243.16460812
+125K: $/gross kWh = -0.00010551x3 + 0.02954283x2 - 2.89409681x + 218.42199600
+250K: $/gross kWh = -0.00009965x3 + 0.02776430x2 - 2.69776661x + 203.67861255
+450K: $/gross kWh = -0.00009556x3 + 0.02652171x2 - 2.56085176x + 193.19055124
+Where x is gross kWh.
+For Wh/kg (if you need that for figuring battery weight):
+Wh/kg = 0.0000000847x3 – 0.0000249011 x2 + 0.0023686408 + 0.1245668155
+Where x is gross kWh.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="285">
   <si>
     <t>Markup</t>
   </si>
@@ -923,7 +968,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1043,6 +1088,19 @@
       <color rgb="FFFA7D00"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1535,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1631,7 @@
         <v>216</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1597,7 +1655,7 @@
         <v>211</v>
       </c>
       <c r="B7" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1618,7 +1676,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,6 +1766,101 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689D00CC-D75A-4DA9-B2EA-0CA83BEECCA6}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="4">
+        <f>Markup*C2</f>
+        <v>5.25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.92137184639529734</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.6731590931770557</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5.0622639824789006</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="4">
+        <f>Markup*C3</f>
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.6489597300215004</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3.9424165615843103</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.6185681065433597</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE94D6-2983-4058-A10D-F319D379B239}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -2000,7 +2153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B9F0F9-D24F-4187-97FF-36498970686A}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -2373,7 +2526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F4307-4CCE-4E39-8D04-CE4F082A04BF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2432,7 +2585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1C16C4-514C-4855-AC00-5CBAF6F7CA67}">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -4710,13 +4863,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ACC5D0-181B-4F4E-94F7-26883B6AC5A8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4766,19 +4919,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4803,13 +4957,13 @@
         <v>275</v>
       </c>
       <c r="B2" s="1">
-        <v>-1E-4</v>
+        <v>-9.556E-5</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>9.214600000000001E-8</v>
+        <v>8.4699999999999997E-8</v>
       </c>
       <c r="E2" s="1">
         <v>2019</v>
@@ -4820,13 +4974,13 @@
         <v>276</v>
       </c>
       <c r="B3" s="1">
-        <v>2.87E-2</v>
+        <v>2.652171E-2</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>-2.6592166000000003E-5</v>
+        <v>-2.4901100000000001E-5</v>
       </c>
       <c r="E3" s="1">
         <v>2019</v>
@@ -4837,13 +4991,13 @@
         <v>277</v>
       </c>
       <c r="B4" s="1">
-        <v>-2.9371</v>
+        <v>-2.5608517599999998</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>2.4871698290000002E-3</v>
+        <v>2.3686407999999998E-3</v>
       </c>
       <c r="E4" s="1">
         <v>2019</v>
@@ -4854,13 +5008,13 @@
         <v>278</v>
       </c>
       <c r="B5" s="1">
-        <v>236.25</v>
+        <v>193.19055123999999</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>
       </c>
       <c r="D5" s="1">
-        <v>0.121819787094</v>
+        <v>0.1245668155</v>
       </c>
       <c r="E5" s="1">
         <v>2019</v>
@@ -4869,6 +5023,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
alpha_package_costs revisiongs: changed some ETW and Wh/mi values in ALPHA input values in 2020_09_02_14_38_22_2017_Chevy_Bolt_blind_validation_results.csv. Added comments to alpha_package_costs_module_inputs.xlsx to describe settings for high and low bev cost scenarios.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBolon\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86C7397-3E15-4257-9154-007F57A113A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E879297-A4C3-4FC4-BD05-4F6C4A83FFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-19065" yWindow="120" windowWidth="17910" windowHeight="14100" tabRatio="826" activeTab="3" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -96,6 +96,31 @@
 Where x is gross kWh.
 </t>
         </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cost Sensitivities (all with 450K coeffs)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+batt_cost_low, constant = 180 (aiming for approximately 80$/kWh in 2030, from BNF study)
+                      bev learning rate = 0.04
+batt_cost_high, constant = 230 (aiming for approximately 124$/kWh in 2030, from MIT study)
+                      bev learning rate = 0.01
+batt_cost_mid, constant = 193.19055124 (as above)
+                      bev learning rate = 0.025</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -968,7 +993,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,6 +1126,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1593,16 +1625,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -1610,7 +1642,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -1618,7 +1650,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -1626,7 +1658,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -1634,7 +1666,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -1642,7 +1674,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>217</v>
       </c>
@@ -1650,15 +1682,15 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>211</v>
       </c>
       <c r="B7" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>222</v>
       </c>
@@ -1679,16 +1711,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>264</v>
       </c>
@@ -1711,7 +1743,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -1735,7 +1767,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -1773,17 +1805,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>264</v>
       </c>
@@ -1806,7 +1838,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>265</v>
       </c>
@@ -1830,7 +1862,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>266</v>
       </c>
@@ -1868,12 +1900,12 @@
       <selection activeCell="F1" sqref="F1:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>232</v>
       </c>
@@ -1896,7 +1928,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="str">
         <f>CONCATENATE(B2,"_",D2)</f>
         <v>unibody_0</v>
@@ -1921,7 +1953,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
         <f t="shared" ref="A3:A11" si="1">CONCATENATE(B3,"_",D3)</f>
         <v>unibody_5</v>
@@ -1946,7 +1978,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -1971,7 +2003,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -1996,7 +2028,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2021,7 +2053,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2046,7 +2078,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2071,7 +2103,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2096,7 +2128,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2121,7 +2153,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2161,15 +2193,15 @@
       <selection activeCell="F5" sqref="F5:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="9"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="9"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>263</v>
       </c>
@@ -2192,7 +2224,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>C2</f>
         <v>LDB</v>
@@ -2214,7 +2246,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
         <f>C3</f>
         <v>LRRT1</v>
@@ -2237,7 +2269,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
         <f>C4</f>
         <v>LRRT2</v>
@@ -2261,7 +2293,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="str">
         <f t="shared" ref="A5:A14" si="1">CONCATENATE(B5,"_",D5)</f>
         <v>unibody_0</v>
@@ -2286,7 +2318,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_5</v>
@@ -2312,7 +2344,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -2338,7 +2370,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -2364,7 +2396,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2390,7 +2422,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2415,7 +2447,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2441,7 +2473,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2467,7 +2499,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2493,7 +2525,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2534,9 +2566,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>264</v>
       </c>
@@ -2550,7 +2582,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>265</v>
       </c>
@@ -2565,7 +2597,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>266</v>
       </c>
@@ -2593,21 +2625,21 @@
       <selection activeCell="K51" sqref="K51:K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="181.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="181.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2645,7 +2677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>183</v>
       </c>
@@ -2683,7 +2715,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>184</v>
       </c>
@@ -2721,7 +2753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>185</v>
       </c>
@@ -2759,7 +2791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>186</v>
       </c>
@@ -2797,7 +2829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>193</v>
       </c>
@@ -2832,7 +2864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>194</v>
       </c>
@@ -2867,7 +2899,7 @@
         <v>159.27502634351916</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>195</v>
       </c>
@@ -2902,7 +2934,7 @@
         <v>179.18440463645993</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>197</v>
       </c>
@@ -2937,7 +2969,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>198</v>
       </c>
@@ -2972,7 +3004,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>199</v>
       </c>
@@ -3007,7 +3039,7 @@
         <v>367.54500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>200</v>
       </c>
@@ -3042,7 +3074,7 @@
         <v>442.06851256369526</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>205</v>
       </c>
@@ -3080,7 +3112,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>215</v>
       </c>
@@ -3118,7 +3150,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>216</v>
       </c>
@@ -3153,7 +3185,7 @@
         <v>113.57755999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>229</v>
       </c>
@@ -3188,7 +3220,7 @@
         <v>-97.21050000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>230</v>
       </c>
@@ -3223,7 +3255,7 @@
         <v>-220.98500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>241</v>
       </c>
@@ -3258,7 +3290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>265</v>
       </c>
@@ -3293,7 +3325,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>266</v>
       </c>
@@ -3328,7 +3360,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>267</v>
       </c>
@@ -3366,7 +3398,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>268</v>
       </c>
@@ -3404,7 +3436,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>269</v>
       </c>
@@ -3443,7 +3475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>271</v>
       </c>
@@ -3478,7 +3510,7 @@
         <v>-847.59770000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>272</v>
       </c>
@@ -3513,7 +3545,7 @@
         <v>-626.61270000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>273</v>
       </c>
@@ -3548,7 +3580,7 @@
         <v>88.164999999999964</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>274</v>
       </c>
@@ -3583,7 +3615,7 @@
         <v>309.14999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>275</v>
       </c>
@@ -3618,7 +3650,7 @@
         <v>-658.79864999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>276</v>
       </c>
@@ -3653,7 +3685,7 @@
         <v>-437.81365</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>277</v>
       </c>
@@ -3688,7 +3720,7 @@
         <v>541.10772384767472</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>278</v>
       </c>
@@ -3723,7 +3755,7 @@
         <v>188.79966055354828</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>279</v>
       </c>
@@ -3758,7 +3790,7 @@
         <v>-940.23964999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>280</v>
       </c>
@@ -3793,7 +3825,7 @@
         <v>-313.62695000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>281</v>
       </c>
@@ -3828,7 +3860,7 @@
         <v>-265.93770000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>282</v>
       </c>
@@ -3863,7 +3895,7 @@
         <v>360.67500000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>283</v>
       </c>
@@ -3898,7 +3930,7 @@
         <v>592.64179278554764</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>284</v>
       </c>
@@ -3933,7 +3965,7 @@
         <v>-804.40830000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>285</v>
       </c>
@@ -3968,7 +4000,7 @@
         <v>-177.79560000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>286</v>
       </c>
@@ -4003,7 +4035,7 @@
         <v>135.83591145034848</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>287</v>
       </c>
@@ -4038,7 +4070,7 @@
         <v>-722.52935000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>288</v>
       </c>
@@ -4073,7 +4105,7 @@
         <v>-95.91664999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>289</v>
       </c>
@@ -4108,7 +4140,7 @@
         <v>217.71486145034851</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>294</v>
       </c>
@@ -4143,7 +4175,7 @@
         <v>132.72918861960008</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>295</v>
       </c>
@@ -4178,7 +4210,7 @@
         <v>192.45732349841887</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>296</v>
       </c>
@@ -4213,7 +4245,7 @@
         <v>274.95</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>297</v>
       </c>
@@ -4251,7 +4283,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>298</v>
       </c>
@@ -4289,7 +4321,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>300</v>
       </c>
@@ -4327,7 +4359,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>301</v>
       </c>
@@ -4365,7 +4397,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>302</v>
       </c>
@@ -4403,7 +4435,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>314</v>
       </c>
@@ -4435,7 +4467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>315</v>
       </c>
@@ -4467,7 +4499,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>316</v>
       </c>
@@ -4499,7 +4531,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>317</v>
       </c>
@@ -4531,7 +4563,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>320</v>
       </c>
@@ -4563,7 +4595,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>321</v>
       </c>
@@ -4595,7 +4627,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>337</v>
       </c>
@@ -4624,7 +4656,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>338</v>
       </c>
@@ -4653,7 +4685,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>339</v>
       </c>
@@ -4682,7 +4714,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>358</v>
       </c>
@@ -4711,7 +4743,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>359</v>
       </c>
@@ -4740,7 +4772,7 @@
         <v>11.875</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>360</v>
       </c>
@@ -4785,12 +4817,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4801,7 +4833,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -4812,7 +4844,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -4823,7 +4855,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -4834,7 +4866,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +4877,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>231</v>
       </c>
@@ -4867,13 +4899,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -4881,7 +4913,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -4889,7 +4921,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>283</v>
       </c>
@@ -4897,7 +4929,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -4905,7 +4937,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>284</v>
       </c>
@@ -4922,20 +4954,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -4952,7 +4984,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -4969,7 +5001,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>276</v>
       </c>
@@ -4986,7 +5018,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>277</v>
       </c>
@@ -5003,12 +5035,12 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>278</v>
       </c>
       <c r="B5" s="1">
-        <v>193.19055123999999</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>
@@ -5035,9 +5067,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>229</v>
       </c>
@@ -5045,7 +5077,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5053,7 +5085,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5061,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5069,7 +5101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5090,14 +5122,14 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="22.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>212</v>
       </c>
@@ -5111,7 +5143,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>224</v>
       </c>
@@ -5126,7 +5158,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>225</v>
       </c>
@@ -5141,7 +5173,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>226</v>
       </c>
@@ -5156,7 +5188,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>228</v>
       </c>
@@ -5171,7 +5203,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>227</v>
       </c>
@@ -5186,7 +5218,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>233</v>
       </c>
@@ -5201,7 +5233,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>234</v>
       </c>
@@ -5216,7 +5248,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>235</v>
       </c>
@@ -5231,7 +5263,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>236</v>
       </c>
@@ -5246,7 +5278,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>237</v>
       </c>
@@ -5261,7 +5293,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>238</v>
       </c>
@@ -5276,7 +5308,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>239</v>
       </c>
@@ -5291,7 +5323,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>240</v>
       </c>
@@ -5306,7 +5338,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>241</v>
       </c>
@@ -5321,7 +5353,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>242</v>
       </c>
@@ -5336,7 +5368,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>243</v>
       </c>
@@ -5351,7 +5383,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>244</v>
       </c>
@@ -5366,7 +5398,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>245</v>
       </c>
@@ -5381,7 +5413,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>246</v>
       </c>
@@ -5396,7 +5428,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>247</v>
       </c>
@@ -5411,7 +5443,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>248</v>
       </c>
@@ -5426,7 +5458,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>172</v>
       </c>
@@ -5441,7 +5473,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>249</v>
       </c>
@@ -5457,7 +5489,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>250</v>
       </c>
@@ -5473,7 +5505,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>
@@ -5489,7 +5521,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>252</v>
       </c>
@@ -5504,7 +5536,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>271</v>
       </c>
@@ -5519,7 +5551,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>272</v>
       </c>
@@ -5534,7 +5566,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>273</v>
       </c>
@@ -5549,7 +5581,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>274</v>
       </c>
@@ -5577,15 +5609,15 @@
       <selection activeCell="F2" sqref="F2:F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.33203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="21.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>262</v>
       </c>
@@ -5611,7 +5643,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="str">
         <f>CONCATENATE(B2,"_",C2,"_",D2)</f>
         <v>TRX10_FWD_LPW_LRL</v>
@@ -5639,7 +5671,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
         <f t="shared" ref="A3:A7" si="1">CONCATENATE(B3,"_",C3,"_",D3)</f>
         <v>TRX10_FWD_LPW_HRL</v>
@@ -5667,7 +5699,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_LRL</v>
@@ -5695,7 +5727,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_HRL</v>
@@ -5723,7 +5755,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_HPW</v>
@@ -5751,7 +5783,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_Truck</v>
@@ -5779,7 +5811,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="str">
         <f t="shared" ref="A8:A61" si="2">CONCATENATE(B8,"_",C8,"_",D8)</f>
         <v>TRX11_FWD_LPW_LRL</v>
@@ -5808,7 +5840,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_LPW_HRL</v>
@@ -5837,7 +5869,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_LRL</v>
@@ -5866,7 +5898,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_HRL</v>
@@ -5895,7 +5927,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_HPW</v>
@@ -5924,7 +5956,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_Truck</v>
@@ -5953,7 +5985,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_LRL</v>
@@ -5982,7 +6014,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_HRL</v>
@@ -6011,7 +6043,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_LRL</v>
@@ -6040,7 +6072,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_HRL</v>
@@ -6069,7 +6101,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_HPW</v>
@@ -6098,7 +6130,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_Truck</v>
@@ -6127,7 +6159,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_LRL</v>
@@ -6156,7 +6188,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_HRL</v>
@@ -6185,7 +6217,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_LRL</v>
@@ -6214,7 +6246,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_HRL</v>
@@ -6243,7 +6275,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_HPW</v>
@@ -6272,7 +6304,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_Truck</v>
@@ -6301,7 +6333,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_LRL</v>
@@ -6330,7 +6362,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_HRL</v>
@@ -6359,7 +6391,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_LRL</v>
@@ -6388,7 +6420,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_HRL</v>
@@ -6417,7 +6449,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_HPW</v>
@@ -6446,7 +6478,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_Truck</v>
@@ -6475,7 +6507,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="str">
         <f>CONCATENATE(B32,"_",C32,"_",D32)</f>
         <v>TRX10_AWD_LPW_LRL</v>
@@ -6504,7 +6536,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="str">
         <f t="shared" ref="A33:A37" si="4">CONCATENATE(B33,"_",C33,"_",D33)</f>
         <v>TRX10_AWD_LPW_HRL</v>
@@ -6533,7 +6565,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_LRL</v>
@@ -6562,7 +6594,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_HRL</v>
@@ -6591,7 +6623,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_HPW</v>
@@ -6620,7 +6652,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_Truck</v>
@@ -6649,7 +6681,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_LRL</v>
@@ -6678,7 +6710,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_HRL</v>
@@ -6707,7 +6739,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_LRL</v>
@@ -6736,7 +6768,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_HRL</v>
@@ -6765,7 +6797,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_HPW</v>
@@ -6794,7 +6826,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_Truck</v>
@@ -6823,7 +6855,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_LRL</v>
@@ -6852,7 +6884,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_HRL</v>
@@ -6881,7 +6913,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_LRL</v>
@@ -6910,7 +6942,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_HRL</v>
@@ -6939,7 +6971,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_HPW</v>
@@ -6968,7 +7000,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_Truck</v>
@@ -6997,7 +7029,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_LRL</v>
@@ -7026,7 +7058,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_HRL</v>
@@ -7055,7 +7087,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_LRL</v>
@@ -7084,7 +7116,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_HRL</v>
@@ -7113,7 +7145,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_HPW</v>
@@ -7142,7 +7174,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_Truck</v>
@@ -7171,7 +7203,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_LRL</v>
@@ -7200,7 +7232,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_HRL</v>
@@ -7229,7 +7261,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_LRL</v>
@@ -7258,7 +7290,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_HRL</v>
@@ -7287,7 +7319,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_HPW</v>
@@ -7316,7 +7348,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_Truck</v>
@@ -7345,7 +7377,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="str">
         <f>CONCATENATE(B62,"_",C62,"_",D62)</f>
         <v>TRX10_RWD_LPW_LRL</v>
@@ -7374,7 +7406,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="str">
         <f t="shared" ref="A63:A67" si="7">CONCATENATE(B63,"_",C63,"_",D63)</f>
         <v>TRX10_RWD_LPW_HRL</v>
@@ -7403,7 +7435,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_LRL</v>
@@ -7432,7 +7464,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_HRL</v>
@@ -7461,7 +7493,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_HPW</v>
@@ -7490,7 +7522,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_Truck</v>
@@ -7519,7 +7551,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="str">
         <f t="shared" ref="A68:A91" si="9">CONCATENATE(B68,"_",C68,"_",D68)</f>
         <v>TRX11_RWD_LPW_LRL</v>
@@ -7548,7 +7580,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_LPW_HRL</v>
@@ -7577,7 +7609,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_LRL</v>
@@ -7606,7 +7638,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_HRL</v>
@@ -7635,7 +7667,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_HPW</v>
@@ -7664,7 +7696,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_Truck</v>
@@ -7693,7 +7725,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_LRL</v>
@@ -7722,7 +7754,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_HRL</v>
@@ -7751,7 +7783,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_LRL</v>
@@ -7780,7 +7812,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_HRL</v>
@@ -7809,7 +7841,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_HPW</v>
@@ -7838,7 +7870,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_Truck</v>
@@ -7867,7 +7899,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_LRL</v>
@@ -7896,7 +7928,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_HRL</v>
@@ -7925,7 +7957,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_LRL</v>
@@ -7954,7 +7986,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_HRL</v>
@@ -7983,7 +8015,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_HPW</v>
@@ -8012,7 +8044,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_Truck</v>
@@ -8041,7 +8073,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_LRL</v>
@@ -8070,7 +8102,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_HRL</v>
@@ -8099,7 +8131,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_LRL</v>
@@ -8128,7 +8160,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_HRL</v>
@@ -8157,7 +8189,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_HPW</v>
@@ -8186,7 +8218,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_Truck</v>
@@ -8230,13 +8262,13 @@
       <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>180</v>
       </c>
@@ -8250,7 +8282,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8265,7 +8297,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -8280,7 +8312,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -8295,7 +8327,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -8310,7 +8342,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -8325,7 +8357,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -8340,7 +8372,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -8355,7 +8387,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -8370,7 +8402,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -8385,7 +8417,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -8400,7 +8432,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -8415,7 +8447,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>189</v>
       </c>
@@ -8430,7 +8462,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -8445,7 +8477,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -8460,7 +8492,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -8475,7 +8507,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -8491,7 +8523,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>177</v>
       </c>
@@ -8507,7 +8539,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>178</v>
       </c>
@@ -8523,7 +8555,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -8539,7 +8571,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -8555,7 +8587,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -8584,14 +8616,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>253</v>
       </c>
@@ -8611,7 +8643,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>0</v>
       </c>
@@ -8632,7 +8664,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -8654,7 +8686,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Add run_ID and run_description to alpha_package_costs_module_inputs.xlsx on inputs_code worksheet. Add name_id (run_ID and time_stamp) to cost_clouds.csv file and include template header. Add name_id to output folder name and output filenames.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KBolon\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E879297-A4C3-4FC4-BD05-4F6C4A83FFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B77D45-4005-4C10-9D91-6E81F6A1A875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19065" yWindow="120" windowWidth="17910" windowHeight="14100" tabRatio="826" activeTab="3" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -64,6 +64,64 @@
     <author>Sherwood, Todd</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{2D5A0A0C-45EC-49FC-AB08-E027F7D85F7C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sherwood, Todd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The run_ID will be included in the output folder and filenames along with a timestamp.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{BDD43DA7-41BD-478E-B222-6DA439BDFC64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sherwood, Todd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The optional_run_description will not be used in filenames, but this file will be included in the output folder so the description might be helpful.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sherwood, Todd</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C4D4E348-B3CC-4315-8C9C-4D45F7A7FFE0}">
       <text>
         <r>
@@ -72,7 +130,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sherwood, Todd:
 From MSa: 20210406_1732</t>
@@ -82,7 +140,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 For battery cost, at various annual production volumes:
@@ -111,7 +169,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 batt_cost_low, constant = 180 (aiming for approximately 80$/kWh in 2030, from BNF study)
@@ -128,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="288">
   <si>
     <t>Markup</t>
   </si>
@@ -983,6 +1041,15 @@
   </si>
   <si>
     <t>bev_powertrain_markup</t>
+  </si>
+  <si>
+    <t>run_ID</t>
+  </si>
+  <si>
+    <t>optional_run_description</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -993,7 +1060,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1118,14 +1185,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1622,19 +1682,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -1642,64 +1702,81 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B4" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="1">
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>267</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="1">
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B10" s="1">
         <v>1.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1711,16 +1788,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>264</v>
       </c>
@@ -1743,7 +1820,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -1767,7 +1844,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>266</v>
       </c>
@@ -1805,17 +1882,17 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="10.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>264</v>
       </c>
@@ -1838,7 +1915,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>265</v>
       </c>
@@ -1862,7 +1939,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>266</v>
       </c>
@@ -1900,12 +1977,12 @@
       <selection activeCell="F1" sqref="F1:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>232</v>
       </c>
@@ -1928,7 +2005,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="str">
         <f>CONCATENATE(B2,"_",D2)</f>
         <v>unibody_0</v>
@@ -1953,7 +2030,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f t="shared" ref="A3:A11" si="1">CONCATENATE(B3,"_",D3)</f>
         <v>unibody_5</v>
@@ -1978,7 +2055,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -2003,7 +2080,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -2028,7 +2105,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2053,7 +2130,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2078,7 +2155,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2103,7 +2180,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2128,7 +2205,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2153,7 +2230,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2193,15 +2270,15 @@
       <selection activeCell="F5" sqref="F5:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="9"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="9"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>263</v>
       </c>
@@ -2224,7 +2301,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>C2</f>
         <v>LDB</v>
@@ -2246,7 +2323,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f>C3</f>
         <v>LRRT1</v>
@@ -2269,7 +2346,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f>C4</f>
         <v>LRRT2</v>
@@ -2293,7 +2370,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" ref="A5:A14" si="1">CONCATENATE(B5,"_",D5)</f>
         <v>unibody_0</v>
@@ -2318,7 +2395,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_5</v>
@@ -2344,7 +2421,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_10</v>
@@ -2370,7 +2447,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_15</v>
@@ -2396,7 +2473,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>unibody_20</v>
@@ -2422,7 +2499,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_0</v>
@@ -2447,7 +2524,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_5</v>
@@ -2473,7 +2550,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_10</v>
@@ -2499,7 +2576,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_15</v>
@@ -2525,7 +2602,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="str">
         <f t="shared" si="1"/>
         <v>ladder_20</v>
@@ -2566,9 +2643,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>264</v>
       </c>
@@ -2582,7 +2659,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>265</v>
       </c>
@@ -2597,7 +2674,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>266</v>
       </c>
@@ -2625,21 +2702,21 @@
       <selection activeCell="K51" sqref="K51:K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="181.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="181.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2677,7 +2754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>183</v>
       </c>
@@ -2715,7 +2792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>184</v>
       </c>
@@ -2753,7 +2830,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>185</v>
       </c>
@@ -2791,7 +2868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>186</v>
       </c>
@@ -2829,7 +2906,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>193</v>
       </c>
@@ -2864,7 +2941,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>194</v>
       </c>
@@ -2899,7 +2976,7 @@
         <v>159.27502634351916</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>195</v>
       </c>
@@ -2934,7 +3011,7 @@
         <v>179.18440463645993</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>197</v>
       </c>
@@ -2969,7 +3046,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>198</v>
       </c>
@@ -3004,7 +3081,7 @@
         <v>243.88499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>199</v>
       </c>
@@ -3039,7 +3116,7 @@
         <v>367.54500000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>200</v>
       </c>
@@ -3074,7 +3151,7 @@
         <v>442.06851256369526</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>205</v>
       </c>
@@ -3112,7 +3189,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>215</v>
       </c>
@@ -3150,7 +3227,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>216</v>
       </c>
@@ -3185,7 +3262,7 @@
         <v>113.57755999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>229</v>
       </c>
@@ -3220,7 +3297,7 @@
         <v>-97.21050000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>230</v>
       </c>
@@ -3255,7 +3332,7 @@
         <v>-220.98500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>241</v>
       </c>
@@ -3290,7 +3367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>265</v>
       </c>
@@ -3325,7 +3402,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>266</v>
       </c>
@@ -3360,7 +3437,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>267</v>
       </c>
@@ -3398,7 +3475,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>268</v>
       </c>
@@ -3436,7 +3513,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>269</v>
       </c>
@@ -3475,7 +3552,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>271</v>
       </c>
@@ -3510,7 +3587,7 @@
         <v>-847.59770000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>272</v>
       </c>
@@ -3545,7 +3622,7 @@
         <v>-626.61270000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>273</v>
       </c>
@@ -3580,7 +3657,7 @@
         <v>88.164999999999964</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>274</v>
       </c>
@@ -3615,7 +3692,7 @@
         <v>309.14999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>275</v>
       </c>
@@ -3650,7 +3727,7 @@
         <v>-658.79864999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>276</v>
       </c>
@@ -3685,7 +3762,7 @@
         <v>-437.81365</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>277</v>
       </c>
@@ -3720,7 +3797,7 @@
         <v>541.10772384767472</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>278</v>
       </c>
@@ -3755,7 +3832,7 @@
         <v>188.79966055354828</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>279</v>
       </c>
@@ -3790,7 +3867,7 @@
         <v>-940.23964999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>280</v>
       </c>
@@ -3825,7 +3902,7 @@
         <v>-313.62695000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>281</v>
       </c>
@@ -3860,7 +3937,7 @@
         <v>-265.93770000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>282</v>
       </c>
@@ -3895,7 +3972,7 @@
         <v>360.67500000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>283</v>
       </c>
@@ -3930,7 +4007,7 @@
         <v>592.64179278554764</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>284</v>
       </c>
@@ -3965,7 +4042,7 @@
         <v>-804.40830000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>285</v>
       </c>
@@ -4000,7 +4077,7 @@
         <v>-177.79560000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>286</v>
       </c>
@@ -4035,7 +4112,7 @@
         <v>135.83591145034848</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>287</v>
       </c>
@@ -4070,7 +4147,7 @@
         <v>-722.52935000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>288</v>
       </c>
@@ -4105,7 +4182,7 @@
         <v>-95.91664999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>289</v>
       </c>
@@ -4140,7 +4217,7 @@
         <v>217.71486145034851</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>294</v>
       </c>
@@ -4175,7 +4252,7 @@
         <v>132.72918861960008</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>295</v>
       </c>
@@ -4210,7 +4287,7 @@
         <v>192.45732349841887</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>296</v>
       </c>
@@ -4245,7 +4322,7 @@
         <v>274.95</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>297</v>
       </c>
@@ -4283,7 +4360,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>298</v>
       </c>
@@ -4321,7 +4398,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>300</v>
       </c>
@@ -4359,7 +4436,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>301</v>
       </c>
@@ -4397,7 +4474,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>302</v>
       </c>
@@ -4435,7 +4512,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>314</v>
       </c>
@@ -4467,7 +4544,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>315</v>
       </c>
@@ -4499,7 +4576,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>316</v>
       </c>
@@ -4531,7 +4608,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>317</v>
       </c>
@@ -4563,7 +4640,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>320</v>
       </c>
@@ -4595,7 +4672,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>321</v>
       </c>
@@ -4627,7 +4704,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>337</v>
       </c>
@@ -4656,7 +4733,7 @@
         <v>462.58</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>338</v>
       </c>
@@ -4685,7 +4762,7 @@
         <v>779.745</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>339</v>
       </c>
@@ -4714,7 +4791,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>358</v>
       </c>
@@ -4743,7 +4820,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>359</v>
       </c>
@@ -4772,7 +4849,7 @@
         <v>11.875</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>360</v>
       </c>
@@ -4817,12 +4894,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4833,7 +4910,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -4844,7 +4921,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>169</v>
       </c>
@@ -4855,7 +4932,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -4866,7 +4943,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4877,7 +4954,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>231</v>
       </c>
@@ -4899,13 +4976,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -4913,7 +4990,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -4921,7 +4998,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>283</v>
       </c>
@@ -4929,7 +5006,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -4937,7 +5014,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>284</v>
       </c>
@@ -4954,20 +5031,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -4984,7 +5061,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>275</v>
       </c>
@@ -5001,7 +5078,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>276</v>
       </c>
@@ -5018,7 +5095,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>277</v>
       </c>
@@ -5035,7 +5112,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>278</v>
       </c>
@@ -5067,9 +5144,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>229</v>
       </c>
@@ -5077,7 +5154,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5085,7 +5162,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5093,7 +5170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5101,7 +5178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5122,14 +5199,14 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="22.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>212</v>
       </c>
@@ -5143,7 +5220,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>224</v>
       </c>
@@ -5158,7 +5235,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>225</v>
       </c>
@@ -5173,7 +5250,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>226</v>
       </c>
@@ -5188,7 +5265,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>228</v>
       </c>
@@ -5203,7 +5280,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>227</v>
       </c>
@@ -5218,7 +5295,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>233</v>
       </c>
@@ -5233,7 +5310,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>234</v>
       </c>
@@ -5248,7 +5325,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>235</v>
       </c>
@@ -5263,7 +5340,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>236</v>
       </c>
@@ -5278,7 +5355,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>237</v>
       </c>
@@ -5293,7 +5370,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>238</v>
       </c>
@@ -5308,7 +5385,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>239</v>
       </c>
@@ -5323,7 +5400,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>240</v>
       </c>
@@ -5338,7 +5415,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>241</v>
       </c>
@@ -5353,7 +5430,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>242</v>
       </c>
@@ -5368,7 +5445,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>243</v>
       </c>
@@ -5383,7 +5460,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>244</v>
       </c>
@@ -5398,7 +5475,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>245</v>
       </c>
@@ -5413,7 +5490,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>246</v>
       </c>
@@ -5428,7 +5505,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>247</v>
       </c>
@@ -5443,7 +5520,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>248</v>
       </c>
@@ -5458,7 +5535,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>172</v>
       </c>
@@ -5473,7 +5550,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>249</v>
       </c>
@@ -5489,7 +5566,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>250</v>
       </c>
@@ -5505,7 +5582,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>251</v>
       </c>
@@ -5521,7 +5598,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>252</v>
       </c>
@@ -5536,7 +5613,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>271</v>
       </c>
@@ -5551,7 +5628,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>272</v>
       </c>
@@ -5566,7 +5643,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>273</v>
       </c>
@@ -5581,7 +5658,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>274</v>
       </c>
@@ -5609,15 +5686,15 @@
       <selection activeCell="F2" sqref="F2:F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="21.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>262</v>
       </c>
@@ -5643,7 +5720,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="str">
         <f>CONCATENATE(B2,"_",C2,"_",D2)</f>
         <v>TRX10_FWD_LPW_LRL</v>
@@ -5671,7 +5748,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
         <f t="shared" ref="A3:A7" si="1">CONCATENATE(B3,"_",C3,"_",D3)</f>
         <v>TRX10_FWD_LPW_HRL</v>
@@ -5699,7 +5776,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_LRL</v>
@@ -5727,7 +5804,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_MPW_HRL</v>
@@ -5755,7 +5832,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_HPW</v>
@@ -5783,7 +5860,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
         <f t="shared" si="1"/>
         <v>TRX10_FWD_Truck</v>
@@ -5811,7 +5888,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="str">
         <f t="shared" ref="A8:A61" si="2">CONCATENATE(B8,"_",C8,"_",D8)</f>
         <v>TRX11_FWD_LPW_LRL</v>
@@ -5840,7 +5917,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_LPW_HRL</v>
@@ -5869,7 +5946,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_LRL</v>
@@ -5898,7 +5975,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_MPW_HRL</v>
@@ -5927,7 +6004,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_HPW</v>
@@ -5956,7 +6033,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_FWD_Truck</v>
@@ -5985,7 +6062,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_LRL</v>
@@ -6014,7 +6091,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_LPW_HRL</v>
@@ -6043,7 +6120,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_LRL</v>
@@ -6072,7 +6149,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_MPW_HRL</v>
@@ -6101,7 +6178,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_HPW</v>
@@ -6130,7 +6207,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_FWD_Truck</v>
@@ -6159,7 +6236,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_LRL</v>
@@ -6188,7 +6265,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_LPW_HRL</v>
@@ -6217,7 +6294,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_LRL</v>
@@ -6246,7 +6323,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_MPW_HRL</v>
@@ -6275,7 +6352,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_HPW</v>
@@ -6304,7 +6381,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_FWD_Truck</v>
@@ -6333,7 +6410,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_LRL</v>
@@ -6362,7 +6439,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_LPW_HRL</v>
@@ -6391,7 +6468,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_LRL</v>
@@ -6420,7 +6497,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_MPW_HRL</v>
@@ -6449,7 +6526,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_HPW</v>
@@ -6478,7 +6555,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_FWD_Truck</v>
@@ -6507,7 +6584,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="str">
         <f>CONCATENATE(B32,"_",C32,"_",D32)</f>
         <v>TRX10_AWD_LPW_LRL</v>
@@ -6536,7 +6613,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="str">
         <f t="shared" ref="A33:A37" si="4">CONCATENATE(B33,"_",C33,"_",D33)</f>
         <v>TRX10_AWD_LPW_HRL</v>
@@ -6565,7 +6642,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_LRL</v>
@@ -6594,7 +6671,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_MPW_HRL</v>
@@ -6623,7 +6700,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_HPW</v>
@@ -6652,7 +6729,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="str">
         <f t="shared" si="4"/>
         <v>TRX10_AWD_Truck</v>
@@ -6681,7 +6758,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_LRL</v>
@@ -6710,7 +6787,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_LPW_HRL</v>
@@ -6739,7 +6816,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_LRL</v>
@@ -6768,7 +6845,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_MPW_HRL</v>
@@ -6797,7 +6874,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_HPW</v>
@@ -6826,7 +6903,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX11_AWD_Truck</v>
@@ -6855,7 +6932,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_LRL</v>
@@ -6884,7 +6961,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_LPW_HRL</v>
@@ -6913,7 +6990,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_LRL</v>
@@ -6942,7 +7019,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_MPW_HRL</v>
@@ -6971,7 +7048,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_HPW</v>
@@ -7000,7 +7077,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX12_AWD_Truck</v>
@@ -7029,7 +7106,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_LRL</v>
@@ -7058,7 +7135,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_LPW_HRL</v>
@@ -7087,7 +7164,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_LRL</v>
@@ -7116,7 +7193,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_MPW_HRL</v>
@@ -7145,7 +7222,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_HPW</v>
@@ -7174,7 +7251,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX21_AWD_Truck</v>
@@ -7203,7 +7280,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_LRL</v>
@@ -7232,7 +7309,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_LPW_HRL</v>
@@ -7261,7 +7338,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_LRL</v>
@@ -7290,7 +7367,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_MPW_HRL</v>
@@ -7319,7 +7396,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_HPW</v>
@@ -7348,7 +7425,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TRX22_AWD_Truck</v>
@@ -7377,7 +7454,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="str">
         <f>CONCATENATE(B62,"_",C62,"_",D62)</f>
         <v>TRX10_RWD_LPW_LRL</v>
@@ -7406,7 +7483,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="str">
         <f t="shared" ref="A63:A67" si="7">CONCATENATE(B63,"_",C63,"_",D63)</f>
         <v>TRX10_RWD_LPW_HRL</v>
@@ -7435,7 +7512,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_LRL</v>
@@ -7464,7 +7541,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_MPW_HRL</v>
@@ -7493,7 +7570,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_HPW</v>
@@ -7522,7 +7599,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="str">
         <f t="shared" si="7"/>
         <v>TRX10_RWD_Truck</v>
@@ -7551,7 +7628,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="str">
         <f t="shared" ref="A68:A91" si="9">CONCATENATE(B68,"_",C68,"_",D68)</f>
         <v>TRX11_RWD_LPW_LRL</v>
@@ -7580,7 +7657,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_LPW_HRL</v>
@@ -7609,7 +7686,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_LRL</v>
@@ -7638,7 +7715,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_MPW_HRL</v>
@@ -7667,7 +7744,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_HPW</v>
@@ -7696,7 +7773,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX11_RWD_Truck</v>
@@ -7725,7 +7802,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_LRL</v>
@@ -7754,7 +7831,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_LPW_HRL</v>
@@ -7783,7 +7860,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_LRL</v>
@@ -7812,7 +7889,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_MPW_HRL</v>
@@ -7841,7 +7918,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_HPW</v>
@@ -7870,7 +7947,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX12_RWD_Truck</v>
@@ -7899,7 +7976,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_LRL</v>
@@ -7928,7 +8005,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_LPW_HRL</v>
@@ -7957,7 +8034,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_LRL</v>
@@ -7986,7 +8063,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_MPW_HRL</v>
@@ -8015,7 +8092,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_HPW</v>
@@ -8044,7 +8121,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX21_RWD_Truck</v>
@@ -8073,7 +8150,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_LRL</v>
@@ -8102,7 +8179,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_LPW_HRL</v>
@@ -8131,7 +8208,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_LRL</v>
@@ -8160,7 +8237,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_MPW_HRL</v>
@@ -8189,7 +8266,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_HPW</v>
@@ -8218,7 +8295,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="str">
         <f t="shared" si="9"/>
         <v>TRX22_RWD_Truck</v>
@@ -8262,13 +8339,13 @@
       <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>180</v>
       </c>
@@ -8282,7 +8359,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8297,7 +8374,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -8312,7 +8389,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -8327,7 +8404,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -8342,7 +8419,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -8357,7 +8434,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -8372,7 +8449,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -8387,7 +8464,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -8402,7 +8479,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -8417,7 +8494,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -8432,7 +8509,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -8447,7 +8524,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>189</v>
       </c>
@@ -8462,7 +8539,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -8477,7 +8554,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -8492,7 +8569,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -8507,7 +8584,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -8523,7 +8600,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>177</v>
       </c>
@@ -8539,7 +8616,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>178</v>
       </c>
@@ -8555,7 +8632,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>179</v>
       </c>
@@ -8571,7 +8648,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -8587,7 +8664,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>175</v>
       </c>
@@ -8616,14 +8693,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="9"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>253</v>
       </c>
@@ -8643,7 +8720,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>0</v>
       </c>
@@ -8664,7 +8741,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -8686,7 +8763,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Add new module make_hev_from_alpha_ice.py to create HEVs from ALPHA ICE packages. This is not part of the alpha_package_costs.py module. If new HEV costs are desired, run this module first and then run alpha_package_costs.py. Add new worksheets to inputs workbook with HEV curves and metrics. Add code to alpha_package_costs.py to calc HEV costs. Simplify alpha_package_costs.py logic in main() and eliminate Ricardo engine from any results.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -8,31 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B77D45-4005-4C10-9D91-6E81F6A1A875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD21F203-A9CA-4176-8F6B-2B4FB47D34AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" activeTab="4" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
     <sheet name="inputs_workbook" sheetId="8" r:id="rId2"/>
-    <sheet name="bev_metrics" sheetId="20" r:id="rId3"/>
-    <sheet name="pev_curves" sheetId="21" r:id="rId4"/>
-    <sheet name="price_class" sheetId="19" r:id="rId5"/>
-    <sheet name="engine" sheetId="18" r:id="rId6"/>
-    <sheet name="trans" sheetId="2" r:id="rId7"/>
-    <sheet name="accessories" sheetId="3" r:id="rId8"/>
-    <sheet name="start-stop" sheetId="5" r:id="rId9"/>
-    <sheet name="weight_ice" sheetId="4" r:id="rId10"/>
-    <sheet name="weight_pev" sheetId="22" r:id="rId11"/>
-    <sheet name="aero" sheetId="6" r:id="rId12"/>
-    <sheet name="nonaero" sheetId="9" r:id="rId13"/>
-    <sheet name="ac" sheetId="17" r:id="rId14"/>
-    <sheet name="et_dmc" sheetId="7" r:id="rId15"/>
+    <sheet name="pev_metrics" sheetId="20" r:id="rId3"/>
+    <sheet name="bev_curves" sheetId="21" r:id="rId4"/>
+    <sheet name="hev_metrics" sheetId="24" r:id="rId5"/>
+    <sheet name="hev_curves" sheetId="23" r:id="rId6"/>
+    <sheet name="price_class" sheetId="19" r:id="rId7"/>
+    <sheet name="engine" sheetId="18" r:id="rId8"/>
+    <sheet name="trans" sheetId="2" r:id="rId9"/>
+    <sheet name="accessories" sheetId="3" r:id="rId10"/>
+    <sheet name="start-stop" sheetId="5" r:id="rId11"/>
+    <sheet name="weight_ice" sheetId="4" r:id="rId12"/>
+    <sheet name="weight_pev" sheetId="22" r:id="rId13"/>
+    <sheet name="aero" sheetId="6" r:id="rId14"/>
+    <sheet name="nonaero" sheetId="9" r:id="rId15"/>
+    <sheet name="ac" sheetId="17" r:id="rId16"/>
+    <sheet name="et_dmc" sheetId="7" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">aero!$B$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">nonaero!$C$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">trans!$A$1:$H$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">aero!$B$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">nonaero!$C$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">trans!$A$1:$H$91</definedName>
     <definedName name="AWD_scaler">inputs_workbook!$B$6</definedName>
     <definedName name="Markup">inputs_workbook!$B$1</definedName>
     <definedName name="Null_4cyl_DMC">inputs_workbook!$B$4</definedName>
@@ -186,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="302">
   <si>
     <t>Markup</t>
   </si>
@@ -800,9 +802,6 @@
     <t>LDB</t>
   </si>
   <si>
-    <t>gap</t>
-  </si>
-  <si>
     <t>LPW_LRL</t>
   </si>
   <si>
@@ -1028,39 +1027,85 @@
     <t>dollars_per_kWh_curve</t>
   </si>
   <si>
-    <t>kWh_per_kg_curve</t>
-  </si>
-  <si>
     <t>dollars_per_kW_curve</t>
   </si>
   <si>
-    <t>usable_soc</t>
-  </si>
-  <si>
-    <t>charging_loss</t>
-  </si>
-  <si>
-    <t>bev_powertrain_markup</t>
-  </si>
-  <si>
     <t>run_ID</t>
   </si>
   <si>
     <t>optional_run_description</t>
   </si>
   <si>
-    <t>test</t>
+    <t>usable_soc_bev</t>
+  </si>
+  <si>
+    <t>charging_loss_bev</t>
+  </si>
+  <si>
+    <t>gap_bev</t>
+  </si>
+  <si>
+    <t>powertrain_markup_bev</t>
+  </si>
+  <si>
+    <t>usable_soc_hev</t>
+  </si>
+  <si>
+    <t>charging_loss_hev</t>
+  </si>
+  <si>
+    <t>gap_hev</t>
+  </si>
+  <si>
+    <t>powertrain_markup_hev</t>
+  </si>
+  <si>
+    <t>usable_soc_phev</t>
+  </si>
+  <si>
+    <t>charging_loss_phev</t>
+  </si>
+  <si>
+    <t>gap_phev</t>
+  </si>
+  <si>
+    <t>powertrain_markup_phev</t>
+  </si>
+  <si>
+    <t>co2_reduction_city_hev</t>
+  </si>
+  <si>
+    <t>co2_reduction_hwy_hev</t>
+  </si>
+  <si>
+    <t>kWh_pack_per_kg_curbwt_curve</t>
+  </si>
+  <si>
+    <t>kW_motor_per_kg_curbwt_curve</t>
+  </si>
+  <si>
+    <t>kWh_pack_per_kg_pack_curve</t>
+  </si>
+  <si>
+    <t>co2_reduction_cycle_hev</t>
+  </si>
+  <si>
+    <t>AddingHEV</t>
+  </si>
+  <si>
+    <t>FIrst take at HEV costs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1194,6 +1239,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1266,7 +1319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1298,8 +1351,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1317,11 +1374,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="14" applyFont="1"/>
     <xf numFmtId="1" fontId="18" fillId="3" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="1" xfId="31" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Accent1 2" xfId="20" xr:uid="{D9FD632B-EF7F-49B6-8440-0774D2DADADB}"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
     <cellStyle name="Calculation 2" xfId="14" xr:uid="{FE108587-6BB1-48C6-A201-65192C808774}"/>
+    <cellStyle name="Calculation 2 2" xfId="33" xr:uid="{271F3B4E-206F-401C-B81A-8EA46F45418D}"/>
     <cellStyle name="Calculation 3" xfId="6" xr:uid="{5274EEA8-4A6C-49CF-911D-0B513965EDE0}"/>
     <cellStyle name="Calculation 4" xfId="24" xr:uid="{E581566A-4310-498D-B20D-DE28C46FA6DF}"/>
     <cellStyle name="Comma 2" xfId="16" xr:uid="{6C404ECA-4D34-4FDB-9417-7D5B37CECF6C}"/>
@@ -1329,9 +1394,11 @@
     <cellStyle name="Currency 2" xfId="13" xr:uid="{675BCA7D-7530-4994-B905-CADA0F721D5F}"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Input 2" xfId="11" xr:uid="{88B890A1-C25D-4F51-BF67-D6C4F98590D3}"/>
+    <cellStyle name="Input 2 2" xfId="32" xr:uid="{508795FB-99F4-4729-8CBB-CFE13932A010}"/>
     <cellStyle name="Input 3" xfId="22" xr:uid="{1B2D7EB3-7741-4480-BD0C-F6ED1317CF77}"/>
     <cellStyle name="Input 4" xfId="5" xr:uid="{AA04B5F3-8D4C-4162-BCAF-2C5E2DBABC82}"/>
     <cellStyle name="Linked Cell 2" xfId="17" xr:uid="{E76B1D5C-B61E-4A12-A6A9-914B9635274E}"/>
+    <cellStyle name="Linked Cell 2 2" xfId="34" xr:uid="{9CDC69F0-4BDB-4E6B-96DF-9997EAD764BB}"/>
     <cellStyle name="Linked Cell 3" xfId="7" xr:uid="{A4E24AE6-00B3-41A9-BD71-207B6B1CFE7F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{BB3C9F31-2AF0-4A34-BF88-C635292282C0}"/>
@@ -1685,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,31 +1763,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" t="s">
         <v>212</v>
-      </c>
-      <c r="B1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
@@ -1728,7 +1795,7 @@
     </row>
     <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="1">
         <v>2050</v>
@@ -1736,7 +1803,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="1">
         <v>5.0000000000000001E-3</v>
@@ -1744,7 +1811,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="1">
         <v>0.01</v>
@@ -1752,7 +1819,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="1">
         <v>1.4999999999999999E-2</v>
@@ -1760,15 +1827,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="1">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10" s="1">
         <v>1.2</v>
@@ -1781,6 +1848,466 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC79EF4-77A1-48AD-8822-597C66753CF5}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <f t="shared" ref="B2:B22" si="0">C2*Markup</f>
+        <v>150</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="1">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" ref="C17:C22" si="1">$C$2+$C$4</f>
+        <v>150</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F0E61-D55E-4846-92CF-DA7BB2817A97}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3800</v>
+      </c>
+      <c r="D2" s="4">
+        <f>E2*Markup</f>
+        <v>481.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>321</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>C2+0.1</f>
+        <v>3800.1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4800</v>
+      </c>
+      <c r="D3" s="4">
+        <f>E3*Markup</f>
+        <v>546</v>
+      </c>
+      <c r="E3" s="1">
+        <v>364</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>C3+0.1</f>
+        <v>4800.1000000000004</v>
+      </c>
+      <c r="C4">
+        <v>8500</v>
+      </c>
+      <c r="D4" s="4">
+        <f>E4*Markup</f>
+        <v>600</v>
+      </c>
+      <c r="E4" s="1">
+        <v>400</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC19E309-23D5-4D0A-B316-FCB0CC8B49A8}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1799,13 +2326,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1817,12 +2344,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2" s="4">
         <f>Markup*C2</f>
@@ -1846,7 +2373,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" s="4">
         <f>Markup*C3</f>
@@ -1874,7 +2401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689D00CC-D75A-4DA9-B2EA-0CA83BEECCA6}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1894,13 +2421,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>7</v>
@@ -1912,12 +2439,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2" s="4">
         <f>Markup*C2</f>
@@ -1941,7 +2468,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" s="4">
         <f>Markup*C3</f>
@@ -1969,7 +2496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE94D6-2983-4058-A10D-F319D379B239}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1984,10 +2511,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -1996,13 +2523,13 @@
         <v>193</v>
       </c>
       <c r="E1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
         <v>171</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2011,7 +2538,7 @@
         <v>unibody_0</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
         <v>194</v>
@@ -2036,7 +2563,7 @@
         <v>unibody_5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -2061,7 +2588,7 @@
         <v>unibody_10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -2086,7 +2613,7 @@
         <v>unibody_15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -2111,7 +2638,7 @@
         <v>unibody_20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -2136,7 +2663,7 @@
         <v>ladder_0</v>
       </c>
       <c r="B7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
         <v>194</v>
@@ -2161,7 +2688,7 @@
         <v>ladder_5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -2186,7 +2713,7 @@
         <v>ladder_10</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -2211,7 +2738,7 @@
         <v>ladder_15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -2236,7 +2763,7 @@
         <v>ladder_20</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -2262,7 +2789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B9F0F9-D24F-4187-97FF-36498970686A}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -2280,10 +2807,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>263</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>264</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -2292,13 +2819,13 @@
         <v>195</v>
       </c>
       <c r="E1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
         <v>171</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2376,7 +2903,7 @@
         <v>unibody_0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" t="s">
         <v>202</v>
@@ -2401,7 +2928,7 @@
         <v>unibody_5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
         <v>198</v>
@@ -2427,7 +2954,7 @@
         <v>unibody_10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
         <v>199</v>
@@ -2453,7 +2980,7 @@
         <v>unibody_15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C8" t="s">
         <v>200</v>
@@ -2479,7 +3006,7 @@
         <v>unibody_20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
         <v>201</v>
@@ -2505,7 +3032,7 @@
         <v>ladder_0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>202</v>
@@ -2530,7 +3057,7 @@
         <v>ladder_5</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>198</v>
@@ -2556,7 +3083,7 @@
         <v>ladder_10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>199</v>
@@ -2582,7 +3109,7 @@
         <v>ladder_15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>200</v>
@@ -2608,7 +3135,7 @@
         <v>ladder_20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>201</v>
@@ -2635,7 +3162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F4307-4CCE-4E39-8D04-CE4F082A04BF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2647,21 +3174,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
         <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2" s="7">
         <f>C2*Markup</f>
@@ -2676,7 +3203,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" s="7">
         <f>C3*Markup</f>
@@ -2694,7 +3221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1C16C4-514C-4855-AC00-5CBAF6F7CA67}">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -2733,7 +3260,7 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
@@ -3156,7 +3683,7 @@
         <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
@@ -3186,7 +3713,7 @@
         <v>13</v>
       </c>
       <c r="L13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -4891,7 +5418,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4907,7 +5434,7 @@
         <v>1.5</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4956,7 +5483,7 @@
     </row>
     <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="1">
         <v>1.2</v>
@@ -4970,24 +5497,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ACC5D0-181B-4F4E-94F7-26883B6AC5A8}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5008,7 +5535,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>284</v>
       </c>
       <c r="B4" s="1">
         <v>0.3</v>
@@ -5016,11 +5543,35 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B5" s="13">
+        <v>285</v>
+      </c>
+      <c r="B5" s="1">
         <v>1.5</v>
       </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5032,38 +5583,38 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>281</v>
-      </c>
       <c r="D1" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B2" s="1">
         <v>-9.556E-5</v>
@@ -5080,7 +5631,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="1">
         <v>2.652171E-2</v>
@@ -5097,7 +5648,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="1">
         <v>-2.5608517599999998</v>
@@ -5114,10 +5665,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="1">
-        <v>180</v>
+        <v>193.19055123999999</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>
@@ -5137,6 +5688,237 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07987B69-2230-4E5F-926C-42312732B1EC}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="13">
+        <f>55/45*B6</f>
+        <v>0.24444444444444446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="13">
+        <f>45/55*B6</f>
+        <v>0.16363636363636366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16EAC8-38E2-4645-A6B8-8BBE98EEE76B}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2017</v>
+      </c>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-250.72</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-1.6215999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2017</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1058.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>119.85</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-13.269</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2017</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A766E56F-5991-40E3-98F7-3876634381DF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -5148,10 +5930,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
         <v>229</v>
-      </c>
-      <c r="B1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5191,7 +5973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790C9274-B2D0-4CB1-A413-BFF03ACE11B8}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -5208,21 +5990,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>171</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B23" si="0">Markup*C2</f>
@@ -5237,7 +6019,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
@@ -5252,7 +6034,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
@@ -5267,7 +6049,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
@@ -5282,7 +6064,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
@@ -5297,7 +6079,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="0"/>
@@ -5312,7 +6094,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="0"/>
@@ -5327,7 +6109,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9" s="7">
         <f t="shared" si="0"/>
@@ -5342,7 +6124,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" si="0"/>
@@ -5357,7 +6139,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="0"/>
@@ -5372,7 +6154,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
@@ -5387,7 +6169,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B13" s="7">
         <f t="shared" si="0"/>
@@ -5402,7 +6184,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" si="0"/>
@@ -5417,7 +6199,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B15" s="7">
         <f t="shared" si="0"/>
@@ -5432,7 +6214,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B16" s="7">
         <f t="shared" si="0"/>
@@ -5447,7 +6229,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B17" s="7">
         <f t="shared" si="0"/>
@@ -5462,7 +6244,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" si="0"/>
@@ -5477,7 +6259,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B19" s="7">
         <f t="shared" si="0"/>
@@ -5492,7 +6274,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B20" s="7">
         <f t="shared" si="0"/>
@@ -5507,7 +6289,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B21" s="7">
         <f t="shared" si="0"/>
@@ -5522,7 +6304,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B22" s="7">
         <f t="shared" si="0"/>
@@ -5552,7 +6334,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B24" s="7">
         <f t="shared" ref="B24:B31" si="1">Markup*C24</f>
@@ -5568,7 +6350,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B25" s="7">
         <f t="shared" si="1"/>
@@ -5584,7 +6366,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B26" s="7">
         <f t="shared" si="1"/>
@@ -5600,7 +6382,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B27" s="7">
         <f t="shared" si="1"/>
@@ -5615,7 +6397,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B28" s="7">
         <f t="shared" si="1"/>
@@ -5630,7 +6412,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B29" s="7">
         <f t="shared" si="1"/>
@@ -5645,7 +6427,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B30" s="7">
         <f t="shared" si="1"/>
@@ -5660,7 +6442,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B31" s="7">
         <f t="shared" si="1"/>
@@ -5678,7 +6460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24394527-83C9-43E1-99B9-F6C50D02F0E0}">
   <dimension ref="A1:H91"/>
   <sheetViews>
@@ -5696,28 +6478,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
         <v>173</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
         <v>171</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -5729,10 +6511,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" ref="E2:E33" si="0">Markup*F2</f>
@@ -5757,10 +6539,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="0"/>
@@ -5785,10 +6567,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
@@ -5813,10 +6595,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
@@ -5841,10 +6623,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
@@ -5869,10 +6651,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
@@ -5894,13 +6676,13 @@
         <v>TRX11_FWD_LPW_LRL</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
@@ -5923,13 +6705,13 @@
         <v>TRX11_FWD_LPW_HRL</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
@@ -5952,13 +6734,13 @@
         <v>TRX11_FWD_MPW_LRL</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
@@ -5981,13 +6763,13 @@
         <v>TRX11_FWD_MPW_HRL</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
@@ -6010,13 +6792,13 @@
         <v>TRX11_FWD_HPW</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
@@ -6039,13 +6821,13 @@
         <v>TRX11_FWD_Truck</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
@@ -6068,13 +6850,13 @@
         <v>TRX12_FWD_LPW_LRL</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
@@ -6097,13 +6879,13 @@
         <v>TRX12_FWD_LPW_HRL</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
@@ -6126,13 +6908,13 @@
         <v>TRX12_FWD_MPW_LRL</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
@@ -6155,13 +6937,13 @@
         <v>TRX12_FWD_MPW_HRL</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
@@ -6184,13 +6966,13 @@
         <v>TRX12_FWD_HPW</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
@@ -6213,13 +6995,13 @@
         <v>TRX12_FWD_Truck</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
@@ -6242,13 +7024,13 @@
         <v>TRX21_FWD_LPW_LRL</v>
       </c>
       <c r="B20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
@@ -6271,13 +7053,13 @@
         <v>TRX21_FWD_LPW_HRL</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
@@ -6300,13 +7082,13 @@
         <v>TRX21_FWD_MPW_LRL</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
@@ -6329,13 +7111,13 @@
         <v>TRX21_FWD_MPW_HRL</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
@@ -6358,13 +7140,13 @@
         <v>TRX21_FWD_HPW</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
@@ -6387,13 +7169,13 @@
         <v>TRX21_FWD_Truck</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
@@ -6416,13 +7198,13 @@
         <v>TRX22_FWD_LPW_LRL</v>
       </c>
       <c r="B26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
@@ -6445,13 +7227,13 @@
         <v>TRX22_FWD_LPW_HRL</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" si="0"/>
@@ -6474,13 +7256,13 @@
         <v>TRX22_FWD_MPW_LRL</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
@@ -6503,13 +7285,13 @@
         <v>TRX22_FWD_MPW_HRL</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="0"/>
@@ -6532,13 +7314,13 @@
         <v>TRX22_FWD_HPW</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="0"/>
@@ -6561,13 +7343,13 @@
         <v>TRX22_FWD_Truck</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="0"/>
@@ -6593,10 +7375,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="0"/>
@@ -6622,10 +7404,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="0"/>
@@ -6651,10 +7433,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" ref="E34:E65" si="5">Markup*F34</f>
@@ -6680,10 +7462,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E35" s="7">
         <f t="shared" si="5"/>
@@ -6709,10 +7491,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="5"/>
@@ -6738,10 +7520,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="5"/>
@@ -6764,13 +7546,13 @@
         <v>TRX11_AWD_LPW_LRL</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E38" s="7">
         <f t="shared" si="5"/>
@@ -6793,13 +7575,13 @@
         <v>TRX11_AWD_LPW_HRL</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E39" s="7">
         <f t="shared" si="5"/>
@@ -6822,13 +7604,13 @@
         <v>TRX11_AWD_MPW_LRL</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="5"/>
@@ -6851,13 +7633,13 @@
         <v>TRX11_AWD_MPW_HRL</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="5"/>
@@ -6880,13 +7662,13 @@
         <v>TRX11_AWD_HPW</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E42" s="7">
         <f t="shared" si="5"/>
@@ -6909,13 +7691,13 @@
         <v>TRX11_AWD_Truck</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E43" s="7">
         <f t="shared" si="5"/>
@@ -6938,13 +7720,13 @@
         <v>TRX12_AWD_LPW_LRL</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="5"/>
@@ -6967,13 +7749,13 @@
         <v>TRX12_AWD_LPW_HRL</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="5"/>
@@ -6996,13 +7778,13 @@
         <v>TRX12_AWD_MPW_LRL</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E46" s="7">
         <f t="shared" si="5"/>
@@ -7025,13 +7807,13 @@
         <v>TRX12_AWD_MPW_HRL</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E47" s="7">
         <f t="shared" si="5"/>
@@ -7054,13 +7836,13 @@
         <v>TRX12_AWD_HPW</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E48" s="7">
         <f t="shared" si="5"/>
@@ -7083,13 +7865,13 @@
         <v>TRX12_AWD_Truck</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E49" s="7">
         <f t="shared" si="5"/>
@@ -7112,13 +7894,13 @@
         <v>TRX21_AWD_LPW_LRL</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E50" s="7">
         <f t="shared" si="5"/>
@@ -7141,13 +7923,13 @@
         <v>TRX21_AWD_LPW_HRL</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E51" s="7">
         <f t="shared" si="5"/>
@@ -7170,13 +7952,13 @@
         <v>TRX21_AWD_MPW_LRL</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E52" s="7">
         <f t="shared" si="5"/>
@@ -7199,13 +7981,13 @@
         <v>TRX21_AWD_MPW_HRL</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E53" s="7">
         <f t="shared" si="5"/>
@@ -7228,13 +8010,13 @@
         <v>TRX21_AWD_HPW</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E54" s="7">
         <f t="shared" si="5"/>
@@ -7257,13 +8039,13 @@
         <v>TRX21_AWD_Truck</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E55" s="7">
         <f t="shared" si="5"/>
@@ -7286,13 +8068,13 @@
         <v>TRX22_AWD_LPW_LRL</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E56" s="7">
         <f t="shared" si="5"/>
@@ -7315,13 +8097,13 @@
         <v>TRX22_AWD_LPW_HRL</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E57" s="7">
         <f t="shared" si="5"/>
@@ -7344,13 +8126,13 @@
         <v>TRX22_AWD_MPW_LRL</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E58" s="7">
         <f t="shared" si="5"/>
@@ -7373,13 +8155,13 @@
         <v>TRX22_AWD_MPW_HRL</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E59" s="7">
         <f t="shared" si="5"/>
@@ -7402,13 +8184,13 @@
         <v>TRX22_AWD_HPW</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E60" s="7">
         <f t="shared" si="5"/>
@@ -7431,13 +8213,13 @@
         <v>TRX22_AWD_Truck</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E61" s="7">
         <f t="shared" si="5"/>
@@ -7463,10 +8245,10 @@
         <v>3</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E62" s="7">
         <f t="shared" si="5"/>
@@ -7492,10 +8274,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E63" s="7">
         <f t="shared" si="5"/>
@@ -7521,10 +8303,10 @@
         <v>3</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E64" s="7">
         <f t="shared" si="5"/>
@@ -7550,10 +8332,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E65" s="7">
         <f t="shared" si="5"/>
@@ -7579,10 +8361,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E66" s="7">
         <f t="shared" ref="E66:E91" si="8">Markup*F66</f>
@@ -7608,10 +8390,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E67" s="7">
         <f t="shared" si="8"/>
@@ -7634,13 +8416,13 @@
         <v>TRX11_RWD_LPW_LRL</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="8"/>
@@ -7663,13 +8445,13 @@
         <v>TRX11_RWD_LPW_HRL</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E69" s="7">
         <f t="shared" si="8"/>
@@ -7692,13 +8474,13 @@
         <v>TRX11_RWD_MPW_LRL</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="8"/>
@@ -7721,13 +8503,13 @@
         <v>TRX11_RWD_MPW_HRL</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E71" s="7">
         <f t="shared" si="8"/>
@@ -7750,13 +8532,13 @@
         <v>TRX11_RWD_HPW</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E72" s="7">
         <f t="shared" si="8"/>
@@ -7779,13 +8561,13 @@
         <v>TRX11_RWD_Truck</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E73" s="7">
         <f t="shared" si="8"/>
@@ -7808,13 +8590,13 @@
         <v>TRX12_RWD_LPW_LRL</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E74" s="7">
         <f t="shared" si="8"/>
@@ -7837,13 +8619,13 @@
         <v>TRX12_RWD_LPW_HRL</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E75" s="7">
         <f t="shared" si="8"/>
@@ -7866,13 +8648,13 @@
         <v>TRX12_RWD_MPW_LRL</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E76" s="7">
         <f t="shared" si="8"/>
@@ -7895,13 +8677,13 @@
         <v>TRX12_RWD_MPW_HRL</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E77" s="7">
         <f t="shared" si="8"/>
@@ -7924,13 +8706,13 @@
         <v>TRX12_RWD_HPW</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E78" s="7">
         <f t="shared" si="8"/>
@@ -7953,13 +8735,13 @@
         <v>TRX12_RWD_Truck</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E79" s="7">
         <f t="shared" si="8"/>
@@ -7982,13 +8764,13 @@
         <v>TRX21_RWD_LPW_LRL</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E80" s="7">
         <f t="shared" si="8"/>
@@ -8011,13 +8793,13 @@
         <v>TRX21_RWD_LPW_HRL</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E81" s="7">
         <f t="shared" si="8"/>
@@ -8040,13 +8822,13 @@
         <v>TRX21_RWD_MPW_LRL</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E82" s="7">
         <f t="shared" si="8"/>
@@ -8069,13 +8851,13 @@
         <v>TRX21_RWD_MPW_HRL</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E83" s="7">
         <f t="shared" si="8"/>
@@ -8098,13 +8880,13 @@
         <v>TRX21_RWD_HPW</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E84" s="7">
         <f t="shared" si="8"/>
@@ -8127,13 +8909,13 @@
         <v>TRX21_RWD_Truck</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E85" s="7">
         <f t="shared" si="8"/>
@@ -8156,13 +8938,13 @@
         <v>TRX22_RWD_LPW_LRL</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E86" s="7">
         <f t="shared" si="8"/>
@@ -8185,13 +8967,13 @@
         <v>TRX22_RWD_LPW_HRL</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E87" s="7">
         <f t="shared" si="8"/>
@@ -8214,13 +8996,13 @@
         <v>TRX22_RWD_MPW_LRL</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E88" s="7">
         <f t="shared" si="8"/>
@@ -8243,13 +9025,13 @@
         <v>TRX22_RWD_MPW_HRL</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E89" s="7">
         <f t="shared" si="8"/>
@@ -8272,13 +9054,13 @@
         <v>TRX22_RWD_HPW</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E90" s="7">
         <f t="shared" si="8"/>
@@ -8301,13 +9083,13 @@
         <v>TRX22_RWD_Truck</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E91" s="7">
         <f t="shared" si="8"/>
@@ -8329,464 +9111,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC79EF4-77A1-48AD-8822-597C66753CF5}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4">
-        <f t="shared" ref="B2:B22" si="0">C2*Markup</f>
-        <v>150</v>
-      </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="C4" s="1">
-        <v>50</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C5" s="1">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C6" s="1">
-        <v>100</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C7" s="1">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C8" s="1">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C9" s="1">
-        <v>100</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C10" s="1">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C11" s="1">
-        <v>100</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C12" s="1">
-        <v>100</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C13" s="1">
-        <v>100</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C14" s="1">
-        <v>100</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C15" s="1">
-        <v>100</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" s="4">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="C16" s="1">
-        <v>100</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" ref="C17:C22" si="1">$C$2+$C$4</f>
-        <v>150</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C20" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="4">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F0E61-D55E-4846-92CF-DA7BB2817A97}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3800</v>
-      </c>
-      <c r="D2" s="4">
-        <f>E2*Markup</f>
-        <v>481.5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>321</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>C2+0.1</f>
-        <v>3800.1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4800</v>
-      </c>
-      <c r="D3" s="4">
-        <f>E3*Markup</f>
-        <v>546</v>
-      </c>
-      <c r="E3" s="1">
-        <v>364</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f>C3+0.1</f>
-        <v>4800.1000000000004</v>
-      </c>
-      <c r="C4">
-        <v>8500</v>
-      </c>
-      <c r="D4" s="4">
-        <f>E4*Markup</f>
-        <v>600</v>
-      </c>
-      <c r="E4" s="1">
-        <v>400</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2015</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add simulated_vehicle_id to output files. Remove alpha_key from simulated_vehicles (formerly cost_clouds) file. Refactor some variables and output filenames. Add new output file with more verbose details. Breaking up alpha_key into separate columns in verbose output file is not yet done.
</commit_message>
<xml_diff>
--- a/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
+++ b/usepa_omega2_preproc/alpha_package_costs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\usepa_omega2_preproc\alpha_package_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD21F203-A9CA-4176-8F6B-2B4FB47D34AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BE786A-DE33-4413-A09D-7D8A99D0D0E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" activeTab="4" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -1090,10 +1090,10 @@
     <t>co2_reduction_cycle_hev</t>
   </si>
   <si>
-    <t>AddingHEV</t>
-  </si>
-  <si>
-    <t>FIrst take at HEV costs.</t>
+    <t>BEV battery cost curve and learning at mid-range</t>
+  </si>
+  <si>
+    <t>BEV-battery-mid</t>
   </si>
 </sst>
 </file>
@@ -1752,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,7 +1774,7 @@
         <v>280</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1782,7 +1782,7 @@
         <v>281</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5691,7 +5691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07987B69-2230-4E5F-926C-42312732B1EC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>